<commit_message>
ASSIGNED - bug 430514: Add Sphinx serialization generators feature to enable support of XML Persistence Mapping schema generators
https://bugs.eclipse.org/bugs/show_bug.cgi?id=430514

Fixed as proposed.
</commit_message>
<xml_diff>
--- a/docs/org.eclipse.sphinx.doc.design/excel/SphinxFeatureMap.xlsx
+++ b/docs/org.eclipse.sphinx.doc.design/excel/SphinxFeatureMap.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Eclipse\Kepler-SR2\WS-Kepler-SR2\org.eclipse.sphinx\docs\org.eclipse.sphinx.doc.design\excel\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="180" windowWidth="15135" windowHeight="9240"/>
+    <workbookView xWindow="120" yWindow="180" windowWidth="15132" windowHeight="9240"/>
   </bookViews>
   <sheets>
     <sheet name="Root Features" sheetId="4" r:id="rId1"/>
@@ -16,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="129">
   <si>
     <t>Navigator &amp; Editor Sockets</t>
   </si>
@@ -152,9 +157,6 @@
     <t>org.eclipse.sphinx.source</t>
   </si>
   <si>
-    <t>org.eclipse.sphinx.doc.isv</t>
-  </si>
-  <si>
     <t>org.eclipse.sphinx
 org.eclipse.sphinx.source
 org.eclipse.sphinx.doc</t>
@@ -363,16 +365,6 @@
   </si>
   <si>
     <t>Sphinx Auxiliaries</t>
-  </si>
-  <si>
-    <t>org.eclipse.sphinx.core
-org.eclipse.sphinx.emf.editors.forms 
-org.eclipse.sphinx.emf.navigators
-org.eclipse.sphinx.emf.validation
-org.eclipse.sphinx.gmf.editors
-org.eclipse.sphinx.graphiti.editors
-org.eclipse.sphinx.pde
-org.eclipse.sphinx.xtendxpand</t>
   </si>
   <si>
     <t>Sphinx Nebula Extensions Runtime</t>
@@ -425,6 +417,50 @@
 org.eclipse.sphinx.examples.hummingbird20.ide.ui
 org.eclipse.sphinx.examples.hummingbird20.transform.xtend.newwizard
 org.eclipse.sphinx.examples.hummingbird20.validation</t>
+  </si>
+  <si>
+    <t>XML Persistence Mapping</t>
+  </si>
+  <si>
+    <t xml:space="preserve">XML Persistence Mapping based EMF Serialization </t>
+  </si>
+  <si>
+    <t>XML Persistence Mapping &amp; XSD Schema Generators</t>
+  </si>
+  <si>
+    <t>org.eclipse.sphinx.emf.serialization</t>
+  </si>
+  <si>
+    <t>org.eclipse.sphinx.emf.serialization.generators</t>
+  </si>
+  <si>
+    <t>Sphinx XML Persistence Mapping based EMF Serialization</t>
+  </si>
+  <si>
+    <t>Sphinx XML Persistence Mapping &amp; XSD Schema Generators</t>
+  </si>
+  <si>
+    <t>org.eclipse.sphinx.emf.serialization.generators org.eclipse.sphinx.emf.serialization.generators.ui</t>
+  </si>
+  <si>
+    <t>org.eclipse.sphinx.core
+org.eclipse.sphinx.emf.editors.forms 
+org.eclipse.sphinx.emf.navigators
+org.eclipse.sphinx.emf.validation
+org.eclipse.sphinx.gmf.editors
+org.eclipse.sphinx.graphiti.editors
+org.eclipse.sphinx.pde
+org.eclipse.sphinx.xtendxpand org.eclipse.sphinx.emf.serialization org.eclipse.sphinx.emf.serialization.generators</t>
+  </si>
+  <si>
+    <t>Generic serialization/deserialization that extends the EMF XML mappings and allows for configuration of
+persistence mappings on the granularity of individual EStructuralFeatures.</t>
+  </si>
+  <si>
+    <t>XML persistence mapping rules that map between models and XSD schema that covers many existing XML mappings.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">org.eclipse.sphinx.doc.isv </t>
   </si>
 </sst>
 </file>
@@ -587,6 +623,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -607,8 +646,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tableau3" displayName="Tableau3" ref="A1:F9" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
-  <autoFilter ref="A1:F9"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tableau3" displayName="Tableau3" ref="A1:F11" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
+  <autoFilter ref="A1:F11"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Top-level service" dataDxfId="11"/>
     <tableColumn id="2" name="Sub services" dataDxfId="10"/>
@@ -635,7 +674,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -677,7 +716,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -712,7 +751,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -927,209 +966,209 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.5546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.33203125" style="4" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="35" style="4" customWidth="1"/>
-    <col min="4" max="4" width="32.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="47.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="34.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.85546875" style="4"/>
+    <col min="4" max="4" width="32.88671875" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="47.44140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="34.6640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.88671875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>24</v>
       </c>
       <c r="D1" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="E1" s="4" t="s">
-        <v>43</v>
-      </c>
       <c r="F1" s="6" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="102" x14ac:dyDescent="0.2">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="132" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>17</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>107</v>
+        <v>125</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>38</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E3" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="F3" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="F3" s="7" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>39</v>
+        <v>128</v>
       </c>
       <c r="E4" s="4"/>
       <c r="F4" s="7" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>18</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F5" s="7" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A6" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="B6" s="4" t="s">
+      <c r="B8" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="C6" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A7" s="4" t="s">
+      <c r="C8" s="4" t="s">
         <v>103</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="F7" s="7" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A8" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>104</v>
       </c>
       <c r="E8" s="4"/>
       <c r="F8" s="7" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="90.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="90.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>19</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="52.5" customHeight="1" x14ac:dyDescent="0.2">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>20</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>23</v>
       </c>
       <c r="E10" s="4"/>
       <c r="F10" s="7" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="89.25" x14ac:dyDescent="0.2">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="92.4" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>21</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>22</v>
       </c>
       <c r="E11" s="4"/>
       <c r="F11" s="7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
   </sheetData>
@@ -1148,44 +1187,44 @@
   <sheetPr>
     <outlinePr summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView topLeftCell="B4" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="37.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="33.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="45.28515625" style="4" customWidth="1"/>
-    <col min="6" max="6" width="37.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.85546875" style="4"/>
+    <col min="1" max="1" width="26.88671875" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.21875" style="4" customWidth="1"/>
+    <col min="4" max="4" width="33.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="45.33203125" style="4" customWidth="1"/>
+    <col min="6" max="6" width="40.88671875" style="4" customWidth="1"/>
+    <col min="7" max="16384" width="8.88671875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>6</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C1" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>47</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>48</v>
       </c>
       <c r="F1" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
@@ -1196,16 +1235,16 @@
         <v>9</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" ht="52.8" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
         <v>11</v>
       </c>
@@ -1213,30 +1252,30 @@
         <v>7</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F3" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
       <c r="C4" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="D4" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="D4" s="4" t="s">
-        <v>73</v>
-      </c>
       <c r="E4" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="52.8" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
         <v>12</v>
       </c>
@@ -1244,16 +1283,16 @@
         <v>8</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>1</v>
       </c>
@@ -1261,71 +1300,108 @@
         <v>5</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F6" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" ht="66" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>56</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>57</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F7" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
       <c r="C8" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="D8" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="D8" s="4" t="s">
-        <v>75</v>
-      </c>
       <c r="E8" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="87.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="B10" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="87.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B9" s="9" t="s">
-        <v>116</v>
-      </c>
-      <c r="C9" s="4" t="s">
+      <c r="B11" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="C11" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D9" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="F9" s="9" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="F14" s="8"/>
+      <c r="D11" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F16" s="8"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -1345,25 +1421,25 @@
   </sheetPr>
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="47.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="47.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.109375" style="1" customWidth="1"/>
     <col min="3" max="3" width="43" style="1" customWidth="1"/>
-    <col min="4" max="4" width="61.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.85546875" customWidth="1"/>
+    <col min="4" max="4" width="61.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>24</v>
@@ -1373,99 +1449,99 @@
       </c>
       <c r="E1" s="3"/>
     </row>
-    <row r="2" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>31</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>29</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>28</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>27</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="165.75" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" ht="171.6" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>33</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>35</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>36</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>34</v>

</xml_diff>

<commit_message>
RESOLVED - bug 436112: Rework XML Persistence Mapping & XSD generation menu items to make them less prominent in the Eclipse UI https://bugs.eclipse.org/bugs/show_bug.cgi?id=436112
Updated Sphinx feature map
</commit_message>
<xml_diff>
--- a/docs/org.eclipse.sphinx.doc.design/excel/SphinxFeatureMap.xlsx
+++ b/docs/org.eclipse.sphinx.doc.design/excel/SphinxFeatureMap.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Eclipse\Kepler-SR2\WS-Kepler-SR2\org.eclipse.sphinx\docs\org.eclipse.sphinx.doc.design\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\eclipse-sphinx\org.eclipse.sphinx\docs\org.eclipse.sphinx.doc.design\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="180" windowWidth="15132" windowHeight="9240"/>
+    <workbookView xWindow="120" yWindow="180" windowWidth="15135" windowHeight="9240" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Root Features" sheetId="4" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="134">
   <si>
     <t>Navigator &amp; Editor Sockets</t>
   </si>
@@ -270,9 +270,6 @@
     <t>org.eclipse.sphinx.pde</t>
   </si>
   <si>
-    <t>Sphinx PDE</t>
-  </si>
-  <si>
     <t>Extensions of Xtend/Xpand runtime and UI to achieve tight integration with Sphinx workspace management and simplify selection and invocation of Xtend/Xpand/Check templates on Sphinx-managed shared model instances.</t>
   </si>
   <si>
@@ -404,11 +401,76 @@
 org.eclipse.sphinx.platform.ui</t>
   </si>
   <si>
+    <t>XML Persistence Mapping</t>
+  </si>
+  <si>
+    <t xml:space="preserve">XML Persistence Mapping based EMF Serialization </t>
+  </si>
+  <si>
+    <t>XML Persistence Mapping &amp; XSD Schema Generators</t>
+  </si>
+  <si>
+    <t>org.eclipse.sphinx.emf.serialization</t>
+  </si>
+  <si>
+    <t>org.eclipse.sphinx.emf.serialization.generators</t>
+  </si>
+  <si>
+    <t>Sphinx XML Persistence Mapping based EMF Serialization</t>
+  </si>
+  <si>
+    <t>Sphinx XML Persistence Mapping &amp; XSD Schema Generators</t>
+  </si>
+  <si>
+    <t xml:space="preserve">org.eclipse.sphinx.doc.isv </t>
+  </si>
+  <si>
+    <t>org.eclipse.sphinx.core
+org.eclipse.sphinx.emf.editors.forms
+org.eclipse.sphinx.emf.metamodelgen
+org.eclipse.sphinx.emf.navigators
+org.eclipse.sphinx.emf.validation
+org.eclipse.sphinx.gmf.editors
+org.eclipse.sphinx.graphiti.editors
+org.eclipse.sphinx.pde
+org.eclipse.sphinx.xtendxpand org.eclipse.sphinx.emf.serialization org.eclipse.sphinx.emf.serialization.generators</t>
+  </si>
+  <si>
+    <t>Generic serialization/deserialization operating according to XML persistence Mapping annotations on underlying Ecore model. The XML persistence Mapping annotations are defined by Sphinx and extend the ExtendedMetaData annotations supported by EMF. They allow for a very flexible XML mappings of Ecore metamodels on a per-EStructuralFeature basis.</t>
+  </si>
+  <si>
+    <t>Provides generators for automatically adding XML Persistence Mapping annotations to Ecore metamodels and generating a corresponding XSD schema.</t>
+  </si>
+  <si>
+    <t>Metamodel Generation</t>
+  </si>
+  <si>
+    <t>Sphinx Metamodel Generation Tools</t>
+  </si>
+  <si>
+    <t>org.eclipse.sphinx.emf.metamodelgen</t>
+  </si>
+  <si>
+    <t>Provides basic actions, command handlers and operations that are useful for implementing automatic metamodel generation tools.</t>
+  </si>
+  <si>
+    <t>PDE Extensions</t>
+  </si>
+  <si>
+    <t>Sphinx PDE Extensions</t>
+  </si>
+  <si>
+    <t>org.eclipse.sphinx.emf.metamodelgen
+org.eclipse.sphinx.emf.metamodelgen.ui</t>
+  </si>
+  <si>
     <t>org.eclipse.sphinx.examples.hummingbird.ide
 org.eclipse.sphinx.examples.hummingbird.ide.ui
 org.eclipse.sphinx.examples.hummingbird10
 org.eclipse.sphinx.examples.hummingbird10.edit
 org.eclipse.sphinx.examples.hummingbird10.ide.ui
+org.eclipse.sphinx.examples.hummingbird.metamodelgen
+org.eclipse.sphinx.examples.hummingbird.metamodelgen.ui
 org.eclipse.sphinx.examples.hummingbird20
 org.eclipse.sphinx.examples.hummingbird20.codegen.xpand.newwizard
 org.eclipse.sphinx.examples.hummingbird20.diagram.gmf
@@ -417,50 +479,6 @@
 org.eclipse.sphinx.examples.hummingbird20.ide.ui
 org.eclipse.sphinx.examples.hummingbird20.transform.xtend.newwizard
 org.eclipse.sphinx.examples.hummingbird20.validation</t>
-  </si>
-  <si>
-    <t>XML Persistence Mapping</t>
-  </si>
-  <si>
-    <t xml:space="preserve">XML Persistence Mapping based EMF Serialization </t>
-  </si>
-  <si>
-    <t>XML Persistence Mapping &amp; XSD Schema Generators</t>
-  </si>
-  <si>
-    <t>org.eclipse.sphinx.emf.serialization</t>
-  </si>
-  <si>
-    <t>org.eclipse.sphinx.emf.serialization.generators</t>
-  </si>
-  <si>
-    <t>Sphinx XML Persistence Mapping based EMF Serialization</t>
-  </si>
-  <si>
-    <t>Sphinx XML Persistence Mapping &amp; XSD Schema Generators</t>
-  </si>
-  <si>
-    <t>org.eclipse.sphinx.emf.serialization.generators org.eclipse.sphinx.emf.serialization.generators.ui</t>
-  </si>
-  <si>
-    <t>org.eclipse.sphinx.core
-org.eclipse.sphinx.emf.editors.forms 
-org.eclipse.sphinx.emf.navigators
-org.eclipse.sphinx.emf.validation
-org.eclipse.sphinx.gmf.editors
-org.eclipse.sphinx.graphiti.editors
-org.eclipse.sphinx.pde
-org.eclipse.sphinx.xtendxpand org.eclipse.sphinx.emf.serialization org.eclipse.sphinx.emf.serialization.generators</t>
-  </si>
-  <si>
-    <t>Generic serialization/deserialization that extends the EMF XML mappings and allows for configuration of
-persistence mappings on the granularity of individual EStructuralFeatures.</t>
-  </si>
-  <si>
-    <t>XML persistence mapping rules that map between models and XSD schema that covers many existing XML mappings.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">org.eclipse.sphinx.doc.isv </t>
   </si>
 </sst>
 </file>
@@ -548,7 +566,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="22">
     <dxf>
@@ -631,23 +649,23 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tableau2" displayName="Tableau2" ref="A1:F11" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20" headerRowCellStyle="Normal" dataCellStyle="Normal">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tableau2" displayName="Tableau2" ref="A1:F11" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20">
   <autoFilter ref="A1:F11"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="Id" dataDxfId="19" dataCellStyle="Normal"/>
-    <tableColumn id="2" name="Name" dataDxfId="18" dataCellStyle="Normal"/>
-    <tableColumn id="3" name="Description" dataDxfId="17" dataCellStyle="Normal"/>
-    <tableColumn id="4" name="Included plug-ins" dataDxfId="16" dataCellStyle="Normal"/>
-    <tableColumn id="5" name="Included features" dataDxfId="15" dataCellStyle="Normal"/>
-    <tableColumn id="6" name="Update site/p2 repository category" dataDxfId="14" dataCellStyle="Normal"/>
+    <tableColumn id="1" name="Id" dataDxfId="19"/>
+    <tableColumn id="2" name="Name" dataDxfId="18"/>
+    <tableColumn id="3" name="Description" dataDxfId="17"/>
+    <tableColumn id="4" name="Included plug-ins" dataDxfId="16"/>
+    <tableColumn id="5" name="Included features" dataDxfId="15"/>
+    <tableColumn id="6" name="Update site/p2 repository category" dataDxfId="14"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium12" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tableau3" displayName="Tableau3" ref="A1:F11" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
-  <autoFilter ref="A1:F11"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tableau3" displayName="Tableau3" ref="A1:F12" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
+  <autoFilter ref="A1:F12"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Top-level service" dataDxfId="11"/>
     <tableColumn id="2" name="Sub services" dataDxfId="10"/>
@@ -965,22 +983,22 @@
   </sheetPr>
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="28.5546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.28515625" style="4" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="35" style="4" customWidth="1"/>
-    <col min="4" max="4" width="32.88671875" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="47.44140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="34.6640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.88671875" style="4"/>
+    <col min="4" max="4" width="32.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="47.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="34.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.85546875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>44</v>
       </c>
@@ -997,10 +1015,10 @@
         <v>42</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="132" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="140.25" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>17</v>
       </c>
@@ -1008,33 +1026,33 @@
         <v>48</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>38</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>40</v>
       </c>
@@ -1045,14 +1063,14 @@
         <v>54</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="E4" s="4"/>
       <c r="F4" s="7" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="39.6" x14ac:dyDescent="0.25">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>18</v>
       </c>
@@ -1060,65 +1078,65 @@
         <v>50</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>39</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="39.6" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>71</v>
       </c>
       <c r="F6" s="7" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+      <c r="B8" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="C8" s="4" t="s">
         <v>102</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="F7" s="7" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="39.6" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>103</v>
       </c>
       <c r="E8" s="4"/>
       <c r="F8" s="7" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="90.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="90.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>19</v>
       </c>
@@ -1126,16 +1144,16 @@
         <v>51</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>70</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="52.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>20</v>
       </c>
@@ -1143,17 +1161,17 @@
         <v>52</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>23</v>
       </c>
       <c r="E10" s="4"/>
       <c r="F10" s="7" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="92.4" x14ac:dyDescent="0.25">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="89.25" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>21</v>
       </c>
@@ -1161,14 +1179,14 @@
         <v>53</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>22</v>
       </c>
       <c r="E11" s="4"/>
       <c r="F11" s="7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>
@@ -1187,29 +1205,29 @@
   <sheetPr>
     <outlinePr summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView topLeftCell="B4" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="26.88671875" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="38.21875" style="4" customWidth="1"/>
-    <col min="4" max="4" width="33.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="45.33203125" style="4" customWidth="1"/>
-    <col min="6" max="6" width="40.88671875" style="4" customWidth="1"/>
-    <col min="7" max="16384" width="8.88671875" style="4"/>
+    <col min="1" max="1" width="26.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="40" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="45.28515625" style="4" customWidth="1"/>
+    <col min="6" max="6" width="40.85546875" style="4" customWidth="1"/>
+    <col min="7" max="16384" width="8.85546875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>6</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>45</v>
@@ -1224,7 +1242,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="52.8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
@@ -1238,13 +1256,13 @@
         <v>62</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="52.8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="B3" s="4" t="s">
         <v>11</v>
       </c>
@@ -1255,13 +1273,13 @@
         <v>61</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F3" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="C4" s="4" t="s">
         <v>71</v>
       </c>
@@ -1269,13 +1287,13 @@
         <v>72</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F4" s="4" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="52.8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="B5" s="4" t="s">
         <v>12</v>
       </c>
@@ -1286,13 +1304,13 @@
         <v>60</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="39.6" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>1</v>
       </c>
@@ -1303,13 +1321,13 @@
         <v>59</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F6" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="66" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>55</v>
       </c>
@@ -1323,85 +1341,105 @@
         <v>58</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F7" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="B8" s="4" t="s">
+        <v>126</v>
+      </c>
       <c r="C8" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="B9" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="C9" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="D8" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="F8" s="4" t="s">
+      <c r="D9" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="F9" s="4" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="52.8" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+    <row r="10" spans="1:6" ht="102" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+      <c r="B11" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="B9" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="39.6" x14ac:dyDescent="0.25">
-      <c r="B10" s="4" t="s">
+      <c r="C11" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="D11" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="D10" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="87.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
+      <c r="E11" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="87.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B11" s="9" t="s">
+      <c r="B12" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="F12" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="C11" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="F11" s="9" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F16" s="8"/>
+    </row>
+    <row r="17" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F17" s="8"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -1421,20 +1459,20 @@
   </sheetPr>
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="47.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="47.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.140625" style="1" customWidth="1"/>
     <col min="3" max="3" width="43" style="1" customWidth="1"/>
-    <col min="4" max="4" width="61.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.88671875" customWidth="1"/>
+    <col min="4" max="4" width="61.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>44</v>
       </c>
@@ -1449,7 +1487,7 @@
       </c>
       <c r="E1" s="3"/>
     </row>
-    <row r="2" spans="1:5" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>31</v>
       </c>
@@ -1457,13 +1495,13 @@
         <v>63</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>29</v>
       </c>
@@ -1471,13 +1509,13 @@
         <v>65</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="52.8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>28</v>
       </c>
@@ -1485,13 +1523,13 @@
         <v>66</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>27</v>
       </c>
@@ -1499,13 +1537,13 @@
         <v>64</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="171.6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="191.25" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>33</v>
       </c>
@@ -1513,13 +1551,13 @@
         <v>67</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="39.6" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>35</v>
       </c>
@@ -1527,13 +1565,13 @@
         <v>68</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="52.8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>36</v>
       </c>
@@ -1541,7 +1579,7 @@
         <v>69</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>34</v>

</xml_diff>

<commit_message>
Added missing feature names to Sphinx feature map
</commit_message>
<xml_diff>
--- a/docs/org.eclipse.sphinx.doc.design/excel/SphinxFeatureMap.xlsx
+++ b/docs/org.eclipse.sphinx.doc.design/excel/SphinxFeatureMap.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="180" windowWidth="15135" windowHeight="9240" activeTab="2"/>
+    <workbookView xWindow="120" yWindow="180" windowWidth="15135" windowHeight="9240" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Root Features" sheetId="4" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="134">
   <si>
     <t>Navigator &amp; Editor Sockets</t>
   </si>
@@ -208,9 +208,6 @@
   </si>
   <si>
     <t>M2x IDE Integration</t>
-  </si>
-  <si>
-    <t>Xtend/Xpand IDE Integration</t>
   </si>
   <si>
     <t>Sphinx Core</t>
@@ -479,6 +476,9 @@
 org.eclipse.sphinx.examples.hummingbird20.ide.ui
 org.eclipse.sphinx.examples.hummingbird20.transform.xtend.newwizard
 org.eclipse.sphinx.examples.hummingbird20.validation</t>
+  </si>
+  <si>
+    <t>Nebula Nebula Extensions for Form Editors</t>
   </si>
 </sst>
 </file>
@@ -1015,7 +1015,7 @@
         <v>42</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="140.25" x14ac:dyDescent="0.2">
@@ -1026,13 +1026,13 @@
         <v>48</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
@@ -1040,16 +1040,16 @@
         <v>38</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -1063,11 +1063,11 @@
         <v>54</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E4" s="4"/>
       <c r="F4" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
@@ -1078,62 +1078,62 @@
         <v>50</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>39</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E7" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="F7" s="7" t="s">
         <v>110</v>
-      </c>
-      <c r="F7" s="7" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E8" s="4"/>
       <c r="F8" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="90.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1144,13 +1144,13 @@
         <v>51</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="52.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1161,14 +1161,14 @@
         <v>52</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>23</v>
       </c>
       <c r="E10" s="4"/>
       <c r="F10" s="7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="89.25" x14ac:dyDescent="0.2">
@@ -1179,14 +1179,14 @@
         <v>53</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>22</v>
       </c>
       <c r="E11" s="4"/>
       <c r="F11" s="7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
   </sheetData>
@@ -1207,8 +1207,8 @@
   </sheetPr>
   <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView topLeftCell="B4" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1227,7 +1227,7 @@
         <v>6</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>45</v>
@@ -1253,10 +1253,10 @@
         <v>9</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>15</v>
@@ -1270,27 +1270,30 @@
         <v>7</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F3" s="4" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="B4" s="4" t="s">
+        <v>133</v>
+      </c>
       <c r="C4" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D4" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="D4" s="4" t="s">
-        <v>72</v>
-      </c>
       <c r="E4" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="51" x14ac:dyDescent="0.2">
@@ -1301,27 +1304,30 @@
         <v>8</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>1</v>
       </c>
+      <c r="B6" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="C6" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F6" s="4" t="s">
         <v>14</v>
@@ -1332,16 +1338,16 @@
         <v>55</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F7" s="4" t="s">
         <v>16</v>
@@ -1349,73 +1355,73 @@
     </row>
     <row r="8" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
       <c r="B8" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="D8" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="E8" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="D8" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>129</v>
-      </c>
       <c r="F8" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B9" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="D9" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="C9" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>131</v>
-      </c>
       <c r="E9" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="102" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="B10" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="B10" s="4" t="s">
-        <v>116</v>
-      </c>
       <c r="C10" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="B11" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="87.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1423,19 +1429,19 @@
         <v>2</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>3</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="17" spans="6:6" x14ac:dyDescent="0.2">
@@ -1459,7 +1465,7 @@
   </sheetPr>
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
@@ -1492,10 +1498,10 @@
         <v>31</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>32</v>
@@ -1506,10 +1512,10 @@
         <v>29</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>26</v>
@@ -1520,10 +1526,10 @@
         <v>28</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>30</v>
@@ -1534,10 +1540,10 @@
         <v>27</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>25</v>
@@ -1548,13 +1554,13 @@
         <v>33</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
@@ -1562,10 +1568,10 @@
         <v>35</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>37</v>
@@ -1576,10 +1582,10 @@
         <v>36</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>34</v>

</xml_diff>

<commit_message>
ASSIGNED - bug 446340: Add support for dynamic execution of MWE workflows such that workflows can have direct access shared model instances already loaded in Sphinx https://bugs.eclipse.org/bugs/show_bug.cgi?id=446340
Initial implementation
</commit_message>
<xml_diff>
--- a/docs/org.eclipse.sphinx.doc.design/excel/SphinxFeatureMap.xlsx
+++ b/docs/org.eclipse.sphinx.doc.design/excel/SphinxFeatureMap.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\eclipse-sphinx\org.eclipse.sphinx\docs\org.eclipse.sphinx.doc.design\excel\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="120" yWindow="180" windowWidth="15135" windowHeight="9240" activeTab="1"/>
   </bookViews>
@@ -21,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="146">
   <si>
     <t>Navigator &amp; Editor Sockets</t>
   </si>
@@ -249,28 +244,13 @@
     <t>Sphinx Exemplary Extended Library IDE integration</t>
   </si>
   <si>
-    <t>org.eclipse.sphinx.examples.core
-org.eclipse.sphinx.examples.validation
-org.eclipse.sphinx.examples.xtendxpand
-org.eclipse.sphinx.examples.navigators
-org.eclipse.sphinx.examples.metamodels.hummingbird
-org.eclipse.sphinx.examples.metamodels.uml2
-org.eclipse.sphinx.examples.metamodels.library</t>
-  </si>
-  <si>
     <t>org.eclipse.sphinx.emf.editors.forms.nebula</t>
   </si>
   <si>
     <t>Sphinx Nebula Extensions for Form Editors</t>
   </si>
   <si>
-    <t>org.eclipse.sphinx.pde</t>
-  </si>
-  <si>
     <t>Extensions of Xtend/Xpand runtime and UI to achieve tight integration with Sphinx workspace management and simplify selection and invocation of Xtend/Xpand/Check templates on Sphinx-managed shared model instances.</t>
-  </si>
-  <si>
-    <t>Useful extensions of the Plug-in Development Environment runtime.</t>
   </si>
   <si>
     <t>org.eclipse.sphinx.gmf.runtime.ui
@@ -305,9 +285,6 @@
   </si>
   <si>
     <t>Generic Model Explorer view.</t>
-  </si>
-  <si>
-    <t>Hummingbird metamodels and IDE integration including Model Explorer view contribution for Hummingbird content, generic Hummingbird form editor, exemplary graphical Hummingbird editors, exemplary validation services and constraints for Hummingbird, exemplary compare &amp; merge support for Hummingbird, model transformation and code generation examples for Hummingbird, and more.</t>
   </si>
   <si>
     <t>Exemplary UML2 IDE integration including Model Explorer view contribution for UML2 content, and generic UML2 form editor.</t>
@@ -422,17 +399,6 @@
     <t xml:space="preserve">org.eclipse.sphinx.doc.isv </t>
   </si>
   <si>
-    <t>org.eclipse.sphinx.core
-org.eclipse.sphinx.emf.editors.forms
-org.eclipse.sphinx.emf.metamodelgen
-org.eclipse.sphinx.emf.navigators
-org.eclipse.sphinx.emf.validation
-org.eclipse.sphinx.gmf.editors
-org.eclipse.sphinx.graphiti.editors
-org.eclipse.sphinx.pde
-org.eclipse.sphinx.xtendxpand org.eclipse.sphinx.emf.serialization org.eclipse.sphinx.emf.serialization.generators</t>
-  </si>
-  <si>
     <t>Generic serialization/deserialization operating according to XML persistence Mapping annotations on underlying Ecore model. The XML persistence Mapping annotations are defined by Sphinx and extend the ExtendedMetaData annotations supported by EMF. They allow for a very flexible XML mappings of Ecore metamodels on a per-EStructuralFeature basis.</t>
   </si>
   <si>
@@ -449,16 +415,48 @@
   </si>
   <si>
     <t>Provides basic actions, command handlers and operations that are useful for implementing automatic metamodel generation tools.</t>
-  </si>
-  <si>
-    <t>PDE Extensions</t>
-  </si>
-  <si>
-    <t>Sphinx PDE Extensions</t>
   </si>
   <si>
     <t>org.eclipse.sphinx.emf.metamodelgen
 org.eclipse.sphinx.emf.metamodelgen.ui</t>
+  </si>
+  <si>
+    <t>Nebula Extensions for Form Editors</t>
+  </si>
+  <si>
+    <t>org.eclipse.sphinx.emf.mwe.dynamic</t>
+  </si>
+  <si>
+    <t>Scripting Support</t>
+  </si>
+  <si>
+    <t>Dynamic MWE Workflow Support</t>
+  </si>
+  <si>
+    <t>Xtend/Xpand IDE Integration</t>
+  </si>
+  <si>
+    <t>Sphinx Dynamic MWE Workflow Support</t>
+  </si>
+  <si>
+    <t>org.eclipse.sphinx.emf.mwe.dynamic
+org.eclipse.sphinx.emf.mwe.dynamic.headless
+org.eclipse.sphinx.emf.mwe.dynamic.ui</t>
+  </si>
+  <si>
+    <t>Extended runtime-level services allowing users to implement and dynamically execute MWE workflows performing batch manipulations of models or model fragments within the same Eclipse instance.</t>
+  </si>
+  <si>
+    <t>Sphinx Workflow Examples</t>
+  </si>
+  <si>
+    <t>org.eclipse.sphinx.examples.workflows</t>
+  </si>
+  <si>
+    <t>Exemplary MWE workflows that can be imported and dynamically executed in a running Eclipse instance.</t>
+  </si>
+  <si>
+    <t>Hummingbird metamodels and IDE integration including Model Explorer view contribution for Hummingbird content, generic Hummingbird form editor, exemplary graphical Hummingbird editors, exemplary model manipulation workflows for Hummingbird, exemplary validation services and constraints for Hummingbird, model transformation and code generation examples for Hummingbird, and more.</t>
   </si>
   <si>
     <t>org.eclipse.sphinx.examples.hummingbird.ide
@@ -475,10 +473,50 @@
 org.eclipse.sphinx.examples.hummingbird20.editors.nebula
 org.eclipse.sphinx.examples.hummingbird20.ide.ui
 org.eclipse.sphinx.examples.hummingbird20.transform.xtend.newwizard
-org.eclipse.sphinx.examples.hummingbird20.validation</t>
-  </si>
-  <si>
-    <t>Nebula Extensions for Form Editors</t>
+org.eclipse.sphinx.examples.hummingbird20.validation
+org.eclipse.sphinx.examples.hummingbird20.workflows.newwizard</t>
+  </si>
+  <si>
+    <t>org.eclipse.sphinx.examples.core
+org.eclipse.sphinx.examples.metamodels.hummingbird
+org.eclipse.sphinx.examples.metamodels.uml2
+org.eclipse.sphinx.examples.metamodels.library
+org.eclipse.sphinx.examples.navigators
+org.eclipse.sphinx.examples.validation
+org.eclipse.sphinx.examples.workflows
+org.eclipse.sphinx.examples.xtendxpand</t>
+  </si>
+  <si>
+    <t>org.eclipse.sphinx.examples.workflows.lib.newwizard
+org.eclipse.sphinx.examples.workflows.simple.newwizard</t>
+  </si>
+  <si>
+    <t>org.eclipse.sphinx.core
+org.eclipse.sphinx.emf.editors.forms
+org.eclipse.sphinx.emf.metamodelgen
+org.eclipse.sphinx.emf.mwe.dynamic
+org.eclipse.sphinx.emf.navigators
+org.eclipse.sphinx.emf.serialization org.eclipse.sphinx.emf.serialization.generators
+org.eclipse.sphinx.emf.validation
+org.eclipse.sphinx.gmf.editors
+org.eclipse.sphinx.jdtpde
+org.eclipse.sphinx.xtendxpand</t>
+  </si>
+  <si>
+    <t>JDT and PDE Extensions</t>
+  </si>
+  <si>
+    <t>org.eclipse.sphinx.jdtpde</t>
+  </si>
+  <si>
+    <t>Sphinx JDT and PDE Extensions</t>
+  </si>
+  <si>
+    <t>Useful extensions of the Java Development Tooling (JDT) &amp; Plug-in Development Environment (PDE) runtimes.</t>
+  </si>
+  <si>
+    <t>org.eclipse.sphinx.jdt
+org.eclipse.sphinx.pde</t>
   </si>
 </sst>
 </file>
@@ -566,7 +604,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="22">
     <dxf>
@@ -664,8 +702,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tableau3" displayName="Tableau3" ref="A1:F12" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
-  <autoFilter ref="A1:F12"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tableau3" displayName="Tableau3" ref="A1:F13" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
+  <autoFilter ref="A1:F13"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Top-level service" dataDxfId="11"/>
     <tableColumn id="2" name="Sub services" dataDxfId="10"/>
@@ -679,8 +717,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tableau5" displayName="Tableau5" ref="A1:D8" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
-  <autoFilter ref="A1:D8"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tableau5" displayName="Tableau5" ref="A1:D9" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+  <autoFilter ref="A1:D9"/>
   <tableColumns count="4">
     <tableColumn id="1" name="Id" dataDxfId="3"/>
     <tableColumn id="2" name="Name" dataDxfId="2"/>
@@ -692,7 +730,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -734,7 +772,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -769,7 +807,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -984,7 +1022,7 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1015,7 +1053,7 @@
         <v>42</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="140.25" x14ac:dyDescent="0.2">
@@ -1026,13 +1064,13 @@
         <v>48</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>122</v>
+        <v>140</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
@@ -1040,16 +1078,16 @@
         <v>38</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -1063,11 +1101,11 @@
         <v>54</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="E4" s="4"/>
       <c r="F4" s="7" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
@@ -1078,65 +1116,65 @@
         <v>50</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>39</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B7" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="E7" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="C7" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>109</v>
-      </c>
       <c r="F7" s="7" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="E8" s="4"/>
       <c r="F8" s="7" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="90.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="102" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>19</v>
       </c>
@@ -1144,13 +1182,13 @@
         <v>51</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>69</v>
+        <v>138</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="52.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1161,14 +1199,14 @@
         <v>52</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>23</v>
       </c>
       <c r="E10" s="4"/>
       <c r="F10" s="7" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="89.25" x14ac:dyDescent="0.2">
@@ -1179,14 +1217,14 @@
         <v>53</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>22</v>
       </c>
       <c r="E11" s="4"/>
       <c r="F11" s="7" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -1205,19 +1243,19 @@
   <sheetPr>
     <outlinePr summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="26.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.140625" style="4" customWidth="1"/>
     <col min="3" max="3" width="40" style="4" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="33.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="45.28515625" style="4" customWidth="1"/>
+    <col min="5" max="5" width="47.5703125" style="4" customWidth="1"/>
     <col min="6" max="6" width="40.85546875" style="4" customWidth="1"/>
     <col min="7" max="16384" width="8.85546875" style="4"/>
   </cols>
@@ -1227,7 +1265,7 @@
         <v>6</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>45</v>
@@ -1256,13 +1294,16 @@
         <v>61</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>0</v>
+      </c>
       <c r="B3" s="4" t="s">
         <v>11</v>
       </c>
@@ -1273,30 +1314,36 @@
         <v>60</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="F3" s="4" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>0</v>
+      </c>
       <c r="B4" s="4" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="C4" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D4" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="D4" s="4" t="s">
-        <v>71</v>
-      </c>
       <c r="E4" s="4" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>0</v>
+      </c>
       <c r="B5" s="4" t="s">
         <v>12</v>
       </c>
@@ -1307,19 +1354,16 @@
         <v>59</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>1</v>
-      </c>
       <c r="C6" s="4" t="s">
         <v>5</v>
       </c>
@@ -1327,125 +1371,148 @@
         <v>58</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F6" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="C7" s="4" t="s">
+      <c r="B8" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="C8" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D8" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="E8" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="89.25" x14ac:dyDescent="0.2">
+      <c r="A11" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+      <c r="A12" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="87.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="E13" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="F7" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="B8" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="B9" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="102" x14ac:dyDescent="0.2">
-      <c r="A10" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="51" x14ac:dyDescent="0.2">
-      <c r="B11" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="87.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B12" s="9" t="s">
-        <v>112</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="F12" s="9" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="17" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F17" s="8"/>
+      <c r="F13" s="9" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="18" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F18" s="8"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -1463,10 +1530,10 @@
   <sheetPr>
     <outlinePr summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1501,93 +1568,107 @@
         <v>62</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B5" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C5" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="204" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C8" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="51" x14ac:dyDescent="0.2">
-      <c r="A4" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C4" s="4" t="s">
+      <c r="D8" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C9" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="D4" s="4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="191.25" x14ac:dyDescent="0.2">
-      <c r="A6" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A7" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="51" x14ac:dyDescent="0.2">
-      <c r="A8" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="D8" s="4" t="s">
+      <c r="D9" s="4" t="s">
         <v>34</v>
       </c>
     </row>

</xml_diff>

<commit_message>
ASSIGNED - 446340: Add support for dynamic execution of MWE workflows such that workflows can have direct access shared model instances already loaded in Sphinx https://bugs.eclipse.org/bugs/show_bug.cgi?id=446340
Reorganized workflow examples: moved ModelWorkflowExtensions from
Hummingbird 2.0 workflow examples to exemplary workflow library, created
new Extended Library workflow examples
</commit_message>
<xml_diff>
--- a/docs/org.eclipse.sphinx.doc.design/excel/SphinxFeatureMap.xlsx
+++ b/docs/org.eclipse.sphinx.doc.design/excel/SphinxFeatureMap.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\eclipse-sphinx\org.eclipse.sphinx\docs\org.eclipse.sphinx.doc.design\excel\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="180" windowWidth="15135" windowHeight="9240" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="180" windowWidth="15135" windowHeight="9240"/>
   </bookViews>
   <sheets>
     <sheet name="Root Features" sheetId="4" r:id="rId1"/>
@@ -133,10 +138,6 @@
   </si>
   <si>
     <t>org.eclipse.sphinx.examples.metamodels.hummingbird</t>
-  </si>
-  <si>
-    <t>org.eclipse.sphinx.examples.library.ide.newwizard
-org.eclipse.sphinx.examples.library.ide.ui.newwizard</t>
   </si>
   <si>
     <t>org.eclipse.sphinx.examples.metamodels.uml2</t>
@@ -487,10 +488,6 @@
 org.eclipse.sphinx.examples.xtendxpand</t>
   </si>
   <si>
-    <t>org.eclipse.sphinx.examples.workflows.lib.newwizard
-org.eclipse.sphinx.examples.workflows.simple.newwizard</t>
-  </si>
-  <si>
     <t>org.eclipse.sphinx.core
 org.eclipse.sphinx.emf.editors.forms
 org.eclipse.sphinx.emf.metamodelgen
@@ -517,6 +514,15 @@
   <si>
     <t>org.eclipse.sphinx.jdt
 org.eclipse.sphinx.pde</t>
+  </si>
+  <si>
+    <t>org.eclipse.sphinx.examples.library.ide.newwizard
+org.eclipse.sphinx.examples.library.ide.ui.newwizard
+org.eclipse.sphinx.examples.library.workflows.newwizard</t>
+  </si>
+  <si>
+    <t>org.eclipse.sphinx.examples.workflows.newwizard
+org.eclipse.sphinx.examples.workflows.lib.newwizard</t>
   </si>
 </sst>
 </file>
@@ -604,7 +610,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="22">
     <dxf>
@@ -730,7 +736,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -772,7 +778,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -807,7 +813,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1021,8 +1027,8 @@
   </sheetPr>
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1038,22 +1044,22 @@
   <sheetData>
     <row r="1" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>24</v>
       </c>
       <c r="D1" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="E1" s="4" t="s">
-        <v>42</v>
-      </c>
       <c r="F1" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="140.25" x14ac:dyDescent="0.2">
@@ -1061,51 +1067,51 @@
         <v>17</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E4" s="4"/>
       <c r="F4" s="7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
@@ -1113,65 +1119,65 @@
         <v>18</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E7" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="F7" s="7" t="s">
         <v>105</v>
-      </c>
-      <c r="F7" s="7" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E8" s="4"/>
       <c r="F8" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="102" x14ac:dyDescent="0.2">
@@ -1179,16 +1185,16 @@
         <v>19</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="52.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1196,17 +1202,17 @@
         <v>20</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>23</v>
       </c>
       <c r="E10" s="4"/>
       <c r="F10" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="89.25" x14ac:dyDescent="0.2">
@@ -1214,17 +1220,17 @@
         <v>21</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>22</v>
       </c>
       <c r="E11" s="4"/>
       <c r="F11" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -1245,8 +1251,8 @@
   </sheetPr>
   <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1265,16 +1271,16 @@
         <v>6</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C1" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>46</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>47</v>
       </c>
       <c r="F1" s="4" t="s">
         <v>13</v>
@@ -1291,10 +1297,10 @@
         <v>9</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>15</v>
@@ -1311,10 +1317,10 @@
         <v>7</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F3" s="4" t="s">
         <v>7</v>
@@ -1325,19 +1331,19 @@
         <v>0</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C4" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="D4" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="D4" s="4" t="s">
-        <v>70</v>
-      </c>
       <c r="E4" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="51" x14ac:dyDescent="0.2">
@@ -1351,13 +1357,13 @@
         <v>8</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
@@ -1368,10 +1374,10 @@
         <v>5</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F6" s="4" t="s">
         <v>14</v>
@@ -1379,39 +1385,39 @@
     </row>
     <row r="7" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>128</v>
-      </c>
       <c r="C7" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D7" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="F7" s="9" t="s">
         <v>130</v>
-      </c>
-      <c r="E7" s="9" t="s">
-        <v>132</v>
-      </c>
-      <c r="F7" s="9" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F8" s="9" t="s">
         <v>16</v>
@@ -1419,76 +1425,76 @@
     </row>
     <row r="9" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="D9" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="E9" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="D9" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="E9" s="4" t="s">
+      <c r="F9" s="4" t="s">
         <v>123</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="D10" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="E10" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="F10" s="4" t="s">
         <v>143</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>144</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="89.25" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="B11" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="B11" s="4" t="s">
-        <v>111</v>
-      </c>
       <c r="C11" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="87.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1496,19 +1502,19 @@
         <v>2</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>3</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F13" s="9" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="18" spans="6:6" x14ac:dyDescent="0.2">
@@ -1533,7 +1539,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1547,10 +1553,10 @@
   <sheetData>
     <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>24</v>
@@ -1565,10 +1571,10 @@
         <v>31</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>32</v>
@@ -1579,10 +1585,10 @@
         <v>27</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>25</v>
@@ -1590,16 +1596,16 @@
     </row>
     <row r="4" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>135</v>
-      </c>
       <c r="D4" s="4" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
@@ -1607,10 +1613,10 @@
         <v>29</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>26</v>
@@ -1621,10 +1627,10 @@
         <v>28</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>30</v>
@@ -1635,41 +1641,41 @@
         <v>33</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C7" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="D7" s="4" t="s">
         <v>136</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>34</v>
+        <v>144</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated feature map. Added new EMF-IncQuery features.
</commit_message>
<xml_diff>
--- a/docs/org.eclipse.sphinx.doc.design/excel/SphinxFeatureMap.xlsx
+++ b/docs/org.eclipse.sphinx.doc.design/excel/SphinxFeatureMap.xlsx
@@ -1,27 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\eclipse-sphinx\org.eclipse.sphinx\docs\org.eclipse.sphinx.doc.design\excel\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25203"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="180" windowWidth="15135" windowHeight="9240"/>
+    <workbookView xWindow="4020" yWindow="1560" windowWidth="15140" windowHeight="9240"/>
   </bookViews>
   <sheets>
     <sheet name="Root Features" sheetId="4" r:id="rId1"/>
     <sheet name="Component Features" sheetId="1" r:id="rId2"/>
     <sheet name="Example Features" sheetId="5" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="176">
   <si>
     <t>Navigator &amp; Editor Sockets</t>
   </si>
@@ -458,6 +458,86 @@
   </si>
   <si>
     <t>Hummingbird metamodels and IDE integration including Model Explorer view contribution for Hummingbird content, generic Hummingbird form editor, exemplary graphical Hummingbird editors, exemplary model manipulation workflows for Hummingbird, exemplary validation services and constraints for Hummingbird, model transformation and code generation examples for Hummingbird, and more.</t>
+  </si>
+  <si>
+    <t>org.eclipse.sphinx.examples.core
+org.eclipse.sphinx.examples.metamodels.hummingbird
+org.eclipse.sphinx.examples.metamodels.uml2
+org.eclipse.sphinx.examples.metamodels.library
+org.eclipse.sphinx.examples.navigators
+org.eclipse.sphinx.examples.validation
+org.eclipse.sphinx.examples.workflows
+org.eclipse.sphinx.examples.xtendxpand</t>
+  </si>
+  <si>
+    <t>org.eclipse.sphinx.core
+org.eclipse.sphinx.emf.editors.forms
+org.eclipse.sphinx.emf.metamodelgen
+org.eclipse.sphinx.emf.mwe.dynamic
+org.eclipse.sphinx.emf.navigators
+org.eclipse.sphinx.emf.serialization org.eclipse.sphinx.emf.serialization.generators
+org.eclipse.sphinx.emf.validation
+org.eclipse.sphinx.gmf.editors
+org.eclipse.sphinx.jdtpde
+org.eclipse.sphinx.xtendxpand</t>
+  </si>
+  <si>
+    <t>JDT and PDE Extensions</t>
+  </si>
+  <si>
+    <t>org.eclipse.sphinx.jdtpde</t>
+  </si>
+  <si>
+    <t>Sphinx JDT and PDE Extensions</t>
+  </si>
+  <si>
+    <t>Useful extensions of the Java Development Tooling (JDT) &amp; Plug-in Development Environment (PDE) runtimes.</t>
+  </si>
+  <si>
+    <t>org.eclipse.sphinx.jdt
+org.eclipse.sphinx.pde</t>
+  </si>
+  <si>
+    <t>org.eclipse.sphinx.examples.library.ide.newwizard
+org.eclipse.sphinx.examples.library.ide.ui.newwizard
+org.eclipse.sphinx.examples.library.workflows.newwizard</t>
+  </si>
+  <si>
+    <t>org.eclipse.sphinx.examples.workflows.newwizard
+org.eclipse.sphinx.examples.workflows.lib.newwizard</t>
+  </si>
+  <si>
+    <t>org.eclipse.sphinx.incquery</t>
+  </si>
+  <si>
+    <t>org.eclipse.sphinx.incquery.source</t>
+  </si>
+  <si>
+    <t>org.eclipse.sphinx.incquery.sdk</t>
+  </si>
+  <si>
+    <t>org.eclipse.sphinx.examples.incquery</t>
+  </si>
+  <si>
+    <t>org.eclipse.sphinx.examples.hummingbird20.incquery</t>
+  </si>
+  <si>
+    <t>org.eclipse.sphinx.examples.metamodels.hummingbird.incquery</t>
+  </si>
+  <si>
+    <t>Sphinx EMF-IncQuery Examples for Hummingbird Metamodels</t>
+  </si>
+  <si>
+    <t>org.eclipse.sphinx.examples.nebula</t>
+  </si>
+  <si>
+    <t>Sphinx Nebula Extension Examples</t>
+  </si>
+  <si>
+    <t>org.eclipse.sphinx.examples.metamodels.hummingbird.nebula</t>
+  </si>
+  <si>
+    <t>Sphinx Nebula Examples for Hummingbird Metamodels</t>
   </si>
   <si>
     <t>org.eclipse.sphinx.examples.hummingbird.ide
@@ -471,65 +551,76 @@
 org.eclipse.sphinx.examples.hummingbird20.codegen.xpand.newwizard
 org.eclipse.sphinx.examples.hummingbird20.diagram.gmf
 org.eclipse.sphinx.examples.hummingbird20.edit
-org.eclipse.sphinx.examples.hummingbird20.editors.nebula
 org.eclipse.sphinx.examples.hummingbird20.ide.ui
 org.eclipse.sphinx.examples.hummingbird20.transform.xtend.newwizard
 org.eclipse.sphinx.examples.hummingbird20.validation
 org.eclipse.sphinx.examples.hummingbird20.workflows.newwizard</t>
   </si>
   <si>
-    <t>org.eclipse.sphinx.examples.core
-org.eclipse.sphinx.examples.metamodels.hummingbird
-org.eclipse.sphinx.examples.metamodels.uml2
-org.eclipse.sphinx.examples.metamodels.library
-org.eclipse.sphinx.examples.navigators
-org.eclipse.sphinx.examples.validation
-org.eclipse.sphinx.examples.workflows
-org.eclipse.sphinx.examples.xtendxpand</t>
-  </si>
-  <si>
-    <t>org.eclipse.sphinx.core
-org.eclipse.sphinx.emf.editors.forms
-org.eclipse.sphinx.emf.metamodelgen
-org.eclipse.sphinx.emf.mwe.dynamic
-org.eclipse.sphinx.emf.navigators
-org.eclipse.sphinx.emf.serialization org.eclipse.sphinx.emf.serialization.generators
-org.eclipse.sphinx.emf.validation
-org.eclipse.sphinx.gmf.editors
-org.eclipse.sphinx.jdtpde
-org.eclipse.sphinx.xtendxpand</t>
-  </si>
-  <si>
-    <t>JDT and PDE Extensions</t>
-  </si>
-  <si>
-    <t>org.eclipse.sphinx.jdtpde</t>
-  </si>
-  <si>
-    <t>Sphinx JDT and PDE Extensions</t>
-  </si>
-  <si>
-    <t>Useful extensions of the Java Development Tooling (JDT) &amp; Plug-in Development Environment (PDE) runtimes.</t>
-  </si>
-  <si>
-    <t>org.eclipse.sphinx.jdt
-org.eclipse.sphinx.pde</t>
-  </si>
-  <si>
-    <t>org.eclipse.sphinx.examples.library.ide.newwizard
-org.eclipse.sphinx.examples.library.ide.ui.newwizard
-org.eclipse.sphinx.examples.library.workflows.newwizard</t>
-  </si>
-  <si>
-    <t>org.eclipse.sphinx.examples.workflows.newwizard
-org.eclipse.sphinx.examples.workflows.lib.newwizard</t>
+    <t>org.eclipse.sphinx.examples.hummingbird20.editors.nebula</t>
+  </si>
+  <si>
+    <t>Exemplary model queries for Hummindbird metamodels based on EMF-IncQuery.</t>
+  </si>
+  <si>
+    <t>Exemplary Hummingbird form editors with Nebula-based form sections.</t>
+  </si>
+  <si>
+    <t>Sphinx EMF-IncQuery Extension Examples</t>
+  </si>
+  <si>
+    <t>Sphinx EMF-IncQuery Extensions Runtime</t>
+  </si>
+  <si>
+    <t>Sphinx EMF-IncQuery Extensions Source</t>
+  </si>
+  <si>
+    <t>Sphinx EMF-IncQuery Extensions SDK</t>
+  </si>
+  <si>
+    <t>Includes Sphinx EMF-IncQuery Extension Examples (with source code).</t>
+  </si>
+  <si>
+    <t>Includes Sphinx Nebula Extension Examples (with source code).</t>
+  </si>
+  <si>
+    <t>Model Query Support</t>
+  </si>
+  <si>
+    <t>org.eclipse.sphinx.emf.incquery</t>
+  </si>
+  <si>
+    <t>org.eclipse.sphinx.incquery
+org.eclipse.sphinx.incquery.source</t>
+  </si>
+  <si>
+    <t>Source features for all runtime features that are included in org.eclipse.sphinx.incquery</t>
+  </si>
+  <si>
+    <t>Sphinx EMF-IncQuery</t>
+  </si>
+  <si>
+    <t>Sphinx Nebula</t>
+  </si>
+  <si>
+    <t>org.eclipse.sphinx.emf.incquery
+org.eclipse.sphinx.emf.workspace.incquery</t>
+  </si>
+  <si>
+    <t>Includes runtime binaries of Sphinx extensions for EMF-IncQuery (without source code).</t>
+  </si>
+  <si>
+    <t>Includes runtime and source code of Sphinx extensions for EMF-IncQuery.</t>
+  </si>
+  <si>
+    <t>Includes source code of Sphinx extensions for EMF-IncQuery.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -562,16 +653,39 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="11"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE4DFEC"/>
+        <bgColor rgb="FFE4DFEC"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -579,11 +693,78 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFFFFFFF"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFFFFFFF"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFFFFFFF"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFFFFFFF"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -608,9 +789,64 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+  <cellStyles count="53">
+    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="22">
     <dxf>
@@ -693,8 +929,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tableau2" displayName="Tableau2" ref="A1:F11" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20">
-  <autoFilter ref="A1:F11"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tableau2" displayName="Tableau2" ref="A1:F16" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20">
+  <autoFilter ref="A1:F16"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Id" dataDxfId="19"/>
     <tableColumn id="2" name="Name" dataDxfId="18"/>
@@ -708,8 +944,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tableau3" displayName="Tableau3" ref="A1:F13" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
-  <autoFilter ref="A1:F13"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tableau3" displayName="Tableau3" ref="A1:F14" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
+  <autoFilter ref="A1:F14"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Top-level service" dataDxfId="11"/>
     <tableColumn id="2" name="Sub services" dataDxfId="10"/>
@@ -723,8 +959,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tableau5" displayName="Tableau5" ref="A1:D9" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
-  <autoFilter ref="A1:D9"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tableau5" displayName="Tableau5" ref="A1:D11" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+  <autoFilter ref="A1:D11"/>
   <tableColumns count="4">
     <tableColumn id="1" name="Id" dataDxfId="3"/>
     <tableColumn id="2" name="Name" dataDxfId="2"/>
@@ -778,7 +1014,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -813,7 +1049,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1022,27 +1258,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
+  <sheetPr enableFormatConditionsCalculation="0">
     <outlinePr summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="28.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31" style="4" customWidth="1"/>
+    <col min="2" max="2" width="30.33203125" style="4" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="35" style="4" customWidth="1"/>
-    <col min="4" max="4" width="32.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="47.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="34.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.85546875" style="4"/>
+    <col min="4" max="4" width="42.5" style="4" customWidth="1"/>
+    <col min="5" max="5" width="48.83203125" style="6" customWidth="1"/>
+    <col min="6" max="6" width="34.6640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.83203125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" s="5" customFormat="1">
       <c r="A1" s="4" t="s">
         <v>43</v>
       </c>
@@ -1062,7 +1298,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="140.25" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="132">
       <c r="A2" s="4" t="s">
         <v>17</v>
       </c>
@@ -1073,13 +1309,13 @@
         <v>84</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F2" s="7" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" ht="24">
       <c r="A3" s="4" t="s">
         <v>37</v>
       </c>
@@ -1096,7 +1332,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6">
       <c r="A4" s="4" t="s">
         <v>39</v>
       </c>
@@ -1114,7 +1350,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" ht="36">
       <c r="A5" s="4" t="s">
         <v>18</v>
       </c>
@@ -1131,142 +1367,232 @@
         <v>92</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" ht="46" customHeight="1">
       <c r="A6" s="4" t="s">
-        <v>94</v>
+        <v>145</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>99</v>
+        <v>161</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>102</v>
+        <v>173</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>68</v>
+        <v>167</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="46" customHeight="1">
       <c r="A7" s="4" t="s">
-        <v>95</v>
+        <v>146</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>100</v>
+        <v>162</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>97</v>
+        <v>175</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>104</v>
+        <v>169</v>
       </c>
       <c r="F7" s="7" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" ht="46" customHeight="1">
       <c r="A8" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="36">
+      <c r="A9" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="24">
+      <c r="A10" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="36">
+      <c r="A11" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B11" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C11" s="4" t="s">
         <v>96</v>
-      </c>
-      <c r="E8" s="4"/>
-      <c r="F8" s="7" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="102" x14ac:dyDescent="0.2">
-      <c r="A9" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>137</v>
-      </c>
-      <c r="F9" s="7" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="52.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E10" s="4"/>
-      <c r="F10" s="7" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="89.25" x14ac:dyDescent="0.2">
-      <c r="A11" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>22</v>
       </c>
       <c r="E11" s="4"/>
       <c r="F11" s="7" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="96">
+      <c r="A12" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="46" customHeight="1">
+      <c r="A13" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>164</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="46" customHeight="1">
+      <c r="A14" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="52.5" customHeight="1">
+      <c r="A15" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E15" s="4"/>
+      <c r="F15" s="7" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="84">
+      <c r="A16" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E16" s="4"/>
+      <c r="F16" s="7" t="s">
         <v>98</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.78740157499999996" right="0.78740157499999996" top="0.984251969" bottom="0.984251969" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter alignWithMargins="0"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId1"/>
   </tableParts>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
+  <sheetPr enableFormatConditionsCalculation="0">
     <outlinePr summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="26.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.140625" style="4" customWidth="1"/>
+    <col min="1" max="1" width="26.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.1640625" style="4" customWidth="1"/>
     <col min="3" max="3" width="40" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="33.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="47.5703125" style="4" customWidth="1"/>
-    <col min="6" max="6" width="40.85546875" style="4" customWidth="1"/>
-    <col min="7" max="16384" width="8.85546875" style="4"/>
+    <col min="4" max="4" width="33.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="47.5" style="4" customWidth="1"/>
+    <col min="6" max="6" width="40.83203125" style="4" customWidth="1"/>
+    <col min="7" max="16384" width="8.83203125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" s="5" customFormat="1">
       <c r="A1" s="4" t="s">
         <v>6</v>
       </c>
@@ -1286,7 +1612,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="36">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
@@ -1306,7 +1632,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" ht="36">
       <c r="A3" s="4" t="s">
         <v>0</v>
       </c>
@@ -1326,7 +1652,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" ht="24">
       <c r="A4" s="4" t="s">
         <v>0</v>
       </c>
@@ -1346,7 +1672,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" ht="48">
       <c r="A5" s="4" t="s">
         <v>0</v>
       </c>
@@ -1366,7 +1692,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" ht="36">
       <c r="A6" s="4" t="s">
         <v>1</v>
       </c>
@@ -1383,175 +1709,191 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" ht="38" customHeight="1">
       <c r="A7" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="48">
+      <c r="A8" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B8" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C8" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="D7" s="9" t="s">
+      <c r="D8" s="9" t="s">
         <v>129</v>
       </c>
-      <c r="E7" s="9" t="s">
+      <c r="E8" s="9" t="s">
         <v>131</v>
       </c>
-      <c r="F7" s="9" t="s">
+      <c r="F8" s="9" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A8" s="4" t="s">
+    <row r="9" spans="1:6" ht="60">
+      <c r="A9" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B9" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C9" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D9" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="E9" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="F8" s="9" t="s">
+      <c r="F9" s="9" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A9" s="4" t="s">
+    <row r="10" spans="1:6" ht="36">
+      <c r="A10" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C10" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D10" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="E10" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="F9" s="4" t="s">
+      <c r="F10" s="4" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A10" s="4" t="s">
+    <row r="11" spans="1:6" ht="24">
+      <c r="A11" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="C11" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="D11" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="E11" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="F11" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="F10" s="4" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="89.25" x14ac:dyDescent="0.2">
-      <c r="A11" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:6" ht="84">
       <c r="A12" s="4" t="s">
         <v>109</v>
       </c>
       <c r="B12" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="36">
+      <c r="A13" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="B13" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C13" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="D13" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="E12" s="4" t="s">
+      <c r="E13" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="F12" s="4" t="s">
+      <c r="F13" s="4" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="87.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="4" t="s">
+    <row r="14" spans="1:6" ht="87.75" customHeight="1">
+      <c r="A14" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B13" s="9" t="s">
+      <c r="B14" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C14" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="D14" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="E13" s="4" t="s">
+      <c r="E14" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="F13" s="9" t="s">
+      <c r="F14" s="9" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="18" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F18" s="8"/>
+    <row r="19" spans="6:6">
+      <c r="F19" s="8"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.78740157499999996" right="0.78740157499999996" top="0.984251969" bottom="0.984251969" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter alignWithMargins="0"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId1"/>
   </tableParts>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
+  <sheetPr enableFormatConditionsCalculation="0">
     <outlinePr summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="47.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="49.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="31.1640625" style="1" customWidth="1"/>
     <col min="3" max="3" width="43" style="1" customWidth="1"/>
-    <col min="4" max="4" width="61.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.85546875" customWidth="1"/>
+    <col min="4" max="4" width="61.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" s="2" customFormat="1">
       <c r="A1" s="4" t="s">
         <v>43</v>
       </c>
@@ -1566,7 +1908,7 @@
       </c>
       <c r="E1" s="3"/>
     </row>
-    <row r="2" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" ht="24">
       <c r="A2" s="4" t="s">
         <v>31</v>
       </c>
@@ -1580,7 +1922,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5">
       <c r="A3" s="4" t="s">
         <v>27</v>
       </c>
@@ -1594,7 +1936,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" ht="24">
       <c r="A4" s="4" t="s">
         <v>133</v>
       </c>
@@ -1605,10 +1947,10 @@
         <v>134</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="36">
       <c r="A5" s="4" t="s">
         <v>29</v>
       </c>
@@ -1622,7 +1964,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" ht="48">
       <c r="A6" s="4" t="s">
         <v>28</v>
       </c>
@@ -1636,7 +1978,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="204" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" ht="180">
       <c r="A7" s="4" t="s">
         <v>33</v>
       </c>
@@ -1647,44 +1989,77 @@
         <v>135</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="48" customHeight="1">
       <c r="A8" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="32" customHeight="1">
+      <c r="A9" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="42" customHeight="1">
+      <c r="A10" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B10" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C10" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D10" s="4" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="51" x14ac:dyDescent="0.2">
-      <c r="A9" s="4" t="s">
+    <row r="11" spans="1:5" ht="56" customHeight="1">
+      <c r="A11" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B11" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C11" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="D9" s="4" t="s">
-        <v>144</v>
+      <c r="D11" s="4" t="s">
+        <v>143</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.78740157499999996" right="0.78740157499999996" top="0.984251969" bottom="0.984251969" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter alignWithMargins="0"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId1"/>
   </tableParts>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
FIXED Bug 451340 - Check-based Validation Framework. (https://bugs.eclipse.org/bugs/show_bug.cgi?id=451340)
</commit_message>
<xml_diff>
--- a/docs/org.eclipse.sphinx.doc.design/excel/SphinxFeatureMap.xlsx
+++ b/docs/org.eclipse.sphinx.doc.design/excel/SphinxFeatureMap.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25203"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="4020" yWindow="1560" windowWidth="15140" windowHeight="9240"/>
+    <workbookView xWindow="-840" yWindow="-440" windowWidth="28840" windowHeight="18000" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Root Features" sheetId="4" r:id="rId1"/>
@@ -21,12 +21,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="182">
   <si>
     <t>Navigator &amp; Editor Sockets</t>
-  </si>
-  <si>
-    <t>Validation Runtime Extensions</t>
   </si>
   <si>
     <t>Core</t>
@@ -212,9 +209,6 @@
     <t>Sphinx Xtend/Xpand IDE Integration</t>
   </si>
   <si>
-    <t>Sphinx Validation Runtime Extensions</t>
-  </si>
-  <si>
     <t>Sphinx GMF Editor Sockets</t>
   </si>
   <si>
@@ -271,9 +265,6 @@
   </si>
   <si>
     <t>Common logic for GMF-based graphical editors that operate on indiviudal elements of Sphinx-managed shared model instances and integrate into the load/edit/save lifecycle of the same.</t>
-  </si>
-  <si>
-    <t>Extended runtime-level services for validating models or model fragments and visualizing validation results.</t>
   </si>
   <si>
     <t>Includes Sphinx Perspective, exemplary generic model manipulation actions, and more.</t>
@@ -455,9 +446,6 @@
   </si>
   <si>
     <t>Exemplary MWE workflows that can be imported and dynamically executed in a running Eclipse instance.</t>
-  </si>
-  <si>
-    <t>Hummingbird metamodels and IDE integration including Model Explorer view contribution for Hummingbird content, generic Hummingbird form editor, exemplary graphical Hummingbird editors, exemplary model manipulation workflows for Hummingbird, exemplary validation services and constraints for Hummingbird, model transformation and code generation examples for Hummingbird, and more.</t>
   </si>
   <si>
     <t>org.eclipse.sphinx.examples.core
@@ -470,7 +458,138 @@
 org.eclipse.sphinx.examples.xtendxpand</t>
   </si>
   <si>
+    <t>JDT and PDE Extensions</t>
+  </si>
+  <si>
+    <t>org.eclipse.sphinx.jdtpde</t>
+  </si>
+  <si>
+    <t>Sphinx JDT and PDE Extensions</t>
+  </si>
+  <si>
+    <t>Useful extensions of the Java Development Tooling (JDT) &amp; Plug-in Development Environment (PDE) runtimes.</t>
+  </si>
+  <si>
+    <t>org.eclipse.sphinx.jdt
+org.eclipse.sphinx.pde</t>
+  </si>
+  <si>
+    <t>org.eclipse.sphinx.examples.library.ide.newwizard
+org.eclipse.sphinx.examples.library.ide.ui.newwizard
+org.eclipse.sphinx.examples.library.workflows.newwizard</t>
+  </si>
+  <si>
+    <t>org.eclipse.sphinx.examples.workflows.newwizard
+org.eclipse.sphinx.examples.workflows.lib.newwizard</t>
+  </si>
+  <si>
+    <t>org.eclipse.sphinx.incquery</t>
+  </si>
+  <si>
+    <t>org.eclipse.sphinx.incquery.source</t>
+  </si>
+  <si>
+    <t>org.eclipse.sphinx.incquery.sdk</t>
+  </si>
+  <si>
+    <t>org.eclipse.sphinx.examples.incquery</t>
+  </si>
+  <si>
+    <t>org.eclipse.sphinx.examples.hummingbird20.incquery</t>
+  </si>
+  <si>
+    <t>org.eclipse.sphinx.examples.metamodels.hummingbird.incquery</t>
+  </si>
+  <si>
+    <t>Sphinx EMF-IncQuery Examples for Hummingbird Metamodels</t>
+  </si>
+  <si>
+    <t>org.eclipse.sphinx.examples.nebula</t>
+  </si>
+  <si>
+    <t>Sphinx Nebula Extension Examples</t>
+  </si>
+  <si>
+    <t>org.eclipse.sphinx.examples.metamodels.hummingbird.nebula</t>
+  </si>
+  <si>
+    <t>Sphinx Nebula Examples for Hummingbird Metamodels</t>
+  </si>
+  <si>
+    <t>org.eclipse.sphinx.examples.hummingbird20.editors.nebula</t>
+  </si>
+  <si>
+    <t>Exemplary model queries for Hummindbird metamodels based on EMF-IncQuery.</t>
+  </si>
+  <si>
+    <t>Exemplary Hummingbird form editors with Nebula-based form sections.</t>
+  </si>
+  <si>
+    <t>Sphinx EMF-IncQuery Extension Examples</t>
+  </si>
+  <si>
+    <t>Sphinx EMF-IncQuery Extensions Runtime</t>
+  </si>
+  <si>
+    <t>Sphinx EMF-IncQuery Extensions Source</t>
+  </si>
+  <si>
+    <t>Sphinx EMF-IncQuery Extensions SDK</t>
+  </si>
+  <si>
+    <t>Includes Sphinx EMF-IncQuery Extension Examples (with source code).</t>
+  </si>
+  <si>
+    <t>Includes Sphinx Nebula Extension Examples (with source code).</t>
+  </si>
+  <si>
+    <t>Model Query Support</t>
+  </si>
+  <si>
+    <t>org.eclipse.sphinx.emf.incquery</t>
+  </si>
+  <si>
+    <t>org.eclipse.sphinx.incquery
+org.eclipse.sphinx.incquery.source</t>
+  </si>
+  <si>
+    <t>Source features for all runtime features that are included in org.eclipse.sphinx.incquery</t>
+  </si>
+  <si>
+    <t>Sphinx EMF-IncQuery</t>
+  </si>
+  <si>
+    <t>Sphinx Nebula</t>
+  </si>
+  <si>
+    <t>org.eclipse.sphinx.emf.incquery
+org.eclipse.sphinx.emf.workspace.incquery</t>
+  </si>
+  <si>
+    <t>Includes runtime binaries of Sphinx extensions for EMF-IncQuery (without source code).</t>
+  </si>
+  <si>
+    <t>Includes runtime and source code of Sphinx extensions for EMF-IncQuery.</t>
+  </si>
+  <si>
+    <t>Includes source code of Sphinx extensions for EMF-IncQuery.</t>
+  </si>
+  <si>
+    <t>Check Validation</t>
+  </si>
+  <si>
+    <t>org.eclipse.sphinx.emf.check</t>
+  </si>
+  <si>
+    <t>org.eclipse.sphinx.emf.check
+org.eclipse.sphinx.emf.check.catalog
+org.eclipse.sphinx.emf.check.catalog.edit
+org.eclipse.sphinx.emf.check.catalog.editor
+org.eclipse.sphinx.emf.check.ui</t>
+  </si>
+  <si>
     <t>org.eclipse.sphinx.core
+org.eclipse.sphinx.emf.check
 org.eclipse.sphinx.emf.editors.forms
 org.eclipse.sphinx.emf.metamodelgen
 org.eclipse.sphinx.emf.mwe.dynamic
@@ -482,62 +601,22 @@
 org.eclipse.sphinx.xtendxpand</t>
   </si>
   <si>
-    <t>JDT and PDE Extensions</t>
-  </si>
-  <si>
-    <t>org.eclipse.sphinx.jdtpde</t>
-  </si>
-  <si>
-    <t>Sphinx JDT and PDE Extensions</t>
-  </si>
-  <si>
-    <t>Useful extensions of the Java Development Tooling (JDT) &amp; Plug-in Development Environment (PDE) runtimes.</t>
-  </si>
-  <si>
-    <t>org.eclipse.sphinx.jdt
-org.eclipse.sphinx.pde</t>
-  </si>
-  <si>
-    <t>org.eclipse.sphinx.examples.library.ide.newwizard
-org.eclipse.sphinx.examples.library.ide.ui.newwizard
-org.eclipse.sphinx.examples.library.workflows.newwizard</t>
-  </si>
-  <si>
-    <t>org.eclipse.sphinx.examples.workflows.newwizard
-org.eclipse.sphinx.examples.workflows.lib.newwizard</t>
-  </si>
-  <si>
-    <t>org.eclipse.sphinx.incquery</t>
-  </si>
-  <si>
-    <t>org.eclipse.sphinx.incquery.source</t>
-  </si>
-  <si>
-    <t>org.eclipse.sphinx.incquery.sdk</t>
-  </si>
-  <si>
-    <t>org.eclipse.sphinx.examples.incquery</t>
-  </si>
-  <si>
-    <t>org.eclipse.sphinx.examples.hummingbird20.incquery</t>
-  </si>
-  <si>
-    <t>org.eclipse.sphinx.examples.metamodels.hummingbird.incquery</t>
-  </si>
-  <si>
-    <t>Sphinx EMF-IncQuery Examples for Hummingbird Metamodels</t>
-  </si>
-  <si>
-    <t>org.eclipse.sphinx.examples.nebula</t>
-  </si>
-  <si>
-    <t>Sphinx Nebula Extension Examples</t>
-  </si>
-  <si>
-    <t>org.eclipse.sphinx.examples.metamodels.hummingbird.nebula</t>
-  </si>
-  <si>
-    <t>Sphinx Nebula Examples for Hummingbird Metamodels</t>
+    <t>Hummingbird metamodels and IDE integration including Model Explorer view contribution for Hummingbird content, generic Hummingbird form editor, exemplary graphical Hummingbird editors, exemplary model manipulation workflows for Hummingbird, exemplary validation services and constraints for Hummingbird, model transformation, code generation examples for Hummingbird and exemplary check validation and more.</t>
+  </si>
+  <si>
+    <t>Model Validation</t>
+  </si>
+  <si>
+    <t>EMF Validation Runtime Extensions</t>
+  </si>
+  <si>
+    <t>Sphinx EMF Validation Runtime Extensions</t>
+  </si>
+  <si>
+    <t>Extended runtime-level services for validating models or model fragments and visualizing validation results using EMF Validation.</t>
+  </si>
+  <si>
+    <t>Annotation-based framework for validating EMF models.</t>
   </si>
   <si>
     <t>org.eclipse.sphinx.examples.hummingbird.ide
@@ -554,66 +633,11 @@
 org.eclipse.sphinx.examples.hummingbird20.ide.ui
 org.eclipse.sphinx.examples.hummingbird20.transform.xtend.newwizard
 org.eclipse.sphinx.examples.hummingbird20.validation
+org.eclipse.sphinx.examples.hummingbird20.check
 org.eclipse.sphinx.examples.hummingbird20.workflows.newwizard</t>
   </si>
   <si>
-    <t>org.eclipse.sphinx.examples.hummingbird20.editors.nebula</t>
-  </si>
-  <si>
-    <t>Exemplary model queries for Hummindbird metamodels based on EMF-IncQuery.</t>
-  </si>
-  <si>
-    <t>Exemplary Hummingbird form editors with Nebula-based form sections.</t>
-  </si>
-  <si>
-    <t>Sphinx EMF-IncQuery Extension Examples</t>
-  </si>
-  <si>
-    <t>Sphinx EMF-IncQuery Extensions Runtime</t>
-  </si>
-  <si>
-    <t>Sphinx EMF-IncQuery Extensions Source</t>
-  </si>
-  <si>
-    <t>Sphinx EMF-IncQuery Extensions SDK</t>
-  </si>
-  <si>
-    <t>Includes Sphinx EMF-IncQuery Extension Examples (with source code).</t>
-  </si>
-  <si>
-    <t>Includes Sphinx Nebula Extension Examples (with source code).</t>
-  </si>
-  <si>
-    <t>Model Query Support</t>
-  </si>
-  <si>
-    <t>org.eclipse.sphinx.emf.incquery</t>
-  </si>
-  <si>
-    <t>org.eclipse.sphinx.incquery
-org.eclipse.sphinx.incquery.source</t>
-  </si>
-  <si>
-    <t>Source features for all runtime features that are included in org.eclipse.sphinx.incquery</t>
-  </si>
-  <si>
-    <t>Sphinx EMF-IncQuery</t>
-  </si>
-  <si>
-    <t>Sphinx Nebula</t>
-  </si>
-  <si>
-    <t>org.eclipse.sphinx.emf.incquery
-org.eclipse.sphinx.emf.workspace.incquery</t>
-  </si>
-  <si>
-    <t>Includes runtime binaries of Sphinx extensions for EMF-IncQuery (without source code).</t>
-  </si>
-  <si>
-    <t>Includes runtime and source code of Sphinx extensions for EMF-IncQuery.</t>
-  </si>
-  <si>
-    <t>Includes source code of Sphinx extensions for EMF-IncQuery.</t>
+    <t>Sphinx EMF Check Validation</t>
   </si>
 </sst>
 </file>
@@ -709,7 +733,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="53">
+  <cellStyleXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -763,8 +787,28 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -792,8 +836,11 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="53">
+  <cellStyles count="73">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="5" builtinId="8" hidden="1"/>
@@ -820,6 +867,16 @@
     <cellStyle name="Lien hypertexte" xfId="47" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="49" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="71" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="6" builtinId="9" hidden="1"/>
@@ -846,6 +903,16 @@
     <cellStyle name="Lien hypertexte visité" xfId="48" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="50" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="72" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="22">
@@ -944,8 +1011,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tableau3" displayName="Tableau3" ref="A1:F14" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
-  <autoFilter ref="A1:F14"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tableau3" displayName="Tableau3" ref="A1:F15" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
+  <autoFilter ref="A1:F15"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Top-level service" dataDxfId="11"/>
     <tableColumn id="2" name="Sub services" dataDxfId="10"/>
@@ -1263,8 +1330,8 @@
   </sheetPr>
   <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -1280,278 +1347,278 @@
   <sheetData>
     <row r="1" spans="1:6" s="5" customFormat="1">
       <c r="A1" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D1" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="E1" s="4" t="s">
-        <v>41</v>
-      </c>
       <c r="F1" s="6" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="132">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="149" customHeight="1">
       <c r="A2" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>137</v>
+        <v>173</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="24">
       <c r="A3" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="E4" s="4"/>
       <c r="F4" s="7" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="36">
       <c r="A5" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="46" customHeight="1">
       <c r="A6" s="4" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="B6" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="E6" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="C6" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>167</v>
-      </c>
       <c r="F6" s="7" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="46" customHeight="1">
       <c r="A7" s="4" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="46" customHeight="1">
       <c r="A8" s="4" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="36">
       <c r="A9" s="4" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B9" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="C9" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="C9" s="4" t="s">
-        <v>102</v>
-      </c>
       <c r="E9" s="4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="24">
       <c r="A10" s="4" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="36">
       <c r="A11" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="C11" s="4" t="s">
         <v>93</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>96</v>
       </c>
       <c r="E11" s="4"/>
       <c r="F11" s="7" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="96">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="122" customHeight="1">
       <c r="A12" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="46" customHeight="1">
       <c r="A13" s="4" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="C13" s="10" t="s">
+        <v>158</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="F13" s="7" t="s">
         <v>164</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="F13" s="7" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="46" customHeight="1">
       <c r="A14" s="4" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="C14" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="F14" s="7" t="s">
         <v>165</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>154</v>
-      </c>
-      <c r="F14" s="7" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="52.5" customHeight="1">
       <c r="A15" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E15" s="4"/>
       <c r="F15" s="7" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="84">
       <c r="A16" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="D16" s="4" t="s">
         <v>21</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>22</v>
       </c>
       <c r="E16" s="4"/>
       <c r="F16" s="7" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>
@@ -1575,10 +1642,10 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <outlinePr summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -1594,22 +1661,22 @@
   <sheetData>
     <row r="1" spans="1:6" s="5" customFormat="1">
       <c r="A1" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C1" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="E1" s="4" t="s">
-        <v>46</v>
-      </c>
       <c r="F1" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="36">
@@ -1617,19 +1684,19 @@
         <v>0</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="36">
@@ -1637,19 +1704,19 @@
         <v>0</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="24">
@@ -1657,19 +1724,19 @@
         <v>0</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="48">
@@ -1677,185 +1744,208 @@
         <v>0</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="36">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="43" customHeight="1">
       <c r="A6" s="4" t="s">
-        <v>1</v>
+        <v>175</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>176</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>57</v>
+        <v>177</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>77</v>
+        <v>178</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="38" customHeight="1">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="60">
       <c r="A7" s="4" t="s">
-        <v>166</v>
+        <v>175</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>170</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>167</v>
+        <v>171</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>179</v>
       </c>
       <c r="F7" s="4" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="48">
+    <row r="8" spans="1:6" ht="38" customHeight="1">
       <c r="A8" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="48">
+      <c r="A9" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="D9" s="9" t="s">
         <v>126</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="E9" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="F9" s="9" t="s">
         <v>127</v>
       </c>
-      <c r="C8" s="4" t="s">
+    </row>
+    <row r="10" spans="1:6" ht="60">
+      <c r="A10" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B10" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="D8" s="9" t="s">
-        <v>129</v>
-      </c>
-      <c r="E8" s="9" t="s">
-        <v>131</v>
-      </c>
-      <c r="F8" s="9" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="60">
-      <c r="A9" s="4" t="s">
+      <c r="C10" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="36">
+      <c r="A11" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="24">
+      <c r="A12" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="84">
+      <c r="A13" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="36">
+      <c r="A14" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="87.75" customHeight="1">
+      <c r="A15" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D15" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="B9" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="E9" s="4" t="s">
+      <c r="E15" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="F9" s="9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="36">
-      <c r="A10" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="24">
-      <c r="A11" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>139</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="84">
-      <c r="A12" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="36">
-      <c r="A13" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="87.75" customHeight="1">
-      <c r="A14" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B14" s="9" t="s">
-        <v>107</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="F14" s="9" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="19" spans="6:6">
-      <c r="F19" s="8"/>
+      <c r="F15" s="9" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="20" spans="6:6">
+      <c r="F20" s="8"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -1881,7 +1971,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -1895,157 +1985,157 @@
   <sheetData>
     <row r="1" spans="1:5" s="2" customFormat="1">
       <c r="A1" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E1" s="3"/>
     </row>
     <row r="2" spans="1:5" ht="24">
       <c r="A2" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>31</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="24">
       <c r="A4" s="4" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="36">
       <c r="A5" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="48">
       <c r="A6" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="180">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="207" customHeight="1">
       <c r="A7" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>135</v>
+        <v>174</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>156</v>
+        <v>180</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="48" customHeight="1">
       <c r="A8" s="4" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="32" customHeight="1">
       <c r="A9" s="4" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="42" customHeight="1">
       <c r="A10" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="56" customHeight="1">
       <c r="A11" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[FIXED] Bug 449909 - Integration of EMF-Incquery in Sphinx https://bugs.eclipse.org/bugs/show_bug.cgi?id=449909
Added Hummingbird10 and Hummingbird20 Incquery examples.
</commit_message>
<xml_diff>
--- a/docs/org.eclipse.sphinx.doc.design/excel/SphinxFeatureMap.xlsx
+++ b/docs/org.eclipse.sphinx.doc.design/excel/SphinxFeatureMap.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25203"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-840" yWindow="-440" windowWidth="28840" windowHeight="18000" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Root Features" sheetId="4" r:id="rId1"/>
@@ -495,9 +495,6 @@
     <t>org.eclipse.sphinx.examples.incquery</t>
   </si>
   <si>
-    <t>org.eclipse.sphinx.examples.hummingbird20.incquery</t>
-  </si>
-  <si>
     <t>org.eclipse.sphinx.examples.metamodels.hummingbird.incquery</t>
   </si>
   <si>
@@ -638,6 +635,10 @@
   </si>
   <si>
     <t>Sphinx EMF Check Validation</t>
+  </si>
+  <si>
+    <t>org.eclipse.sphinx.examples.hummingbird10.incquery
+org.eclipse.sphinx.examples.hummingbird20.incquery</t>
   </si>
 </sst>
 </file>
@@ -1376,7 +1377,7 @@
         <v>81</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F2" s="7" t="s">
         <v>89</v>
@@ -1439,16 +1440,16 @@
         <v>140</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="46" customHeight="1">
@@ -1456,13 +1457,13 @@
         <v>141</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F7" s="7" t="s">
         <v>102</v>
@@ -1473,16 +1474,16 @@
         <v>142</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="36">
@@ -1499,7 +1500,7 @@
         <v>66</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="24">
@@ -1531,7 +1532,7 @@
       </c>
       <c r="E11" s="4"/>
       <c r="F11" s="7" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="122" customHeight="1">
@@ -1556,33 +1557,33 @@
         <v>143</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="46" customHeight="1">
       <c r="A14" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="B14" s="4" t="s">
         <v>147</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="C14" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="E14" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="C14" s="4" t="s">
-        <v>159</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>149</v>
-      </c>
       <c r="F14" s="7" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="52.5" customHeight="1">
@@ -1644,7 +1645,7 @@
   </sheetPr>
   <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
@@ -1761,19 +1762,19 @@
     </row>
     <row r="6" spans="1:6" ht="43" customHeight="1">
       <c r="A6" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>175</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>176</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D6" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="E6" s="4" t="s">
         <v>177</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>178</v>
       </c>
       <c r="F6" s="4" t="s">
         <v>13</v>
@@ -1781,33 +1782,33 @@
     </row>
     <row r="7" spans="1:6" ht="60">
       <c r="A7" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B7" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>170</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="D7" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="F7" s="4" t="s">
         <v>171</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>181</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>179</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="38" customHeight="1">
       <c r="A8" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="C8" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="C8" s="4" t="s">
-        <v>161</v>
-      </c>
       <c r="F8" s="4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="48">
@@ -1970,8 +1971,8 @@
   </sheetPr>
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -2076,38 +2077,38 @@
         <v>63</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="48" customHeight="1">
       <c r="A8" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="B8" s="4" t="s">
-        <v>146</v>
-      </c>
       <c r="C8" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>144</v>
+        <v>181</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="32" customHeight="1">
       <c r="A9" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="B9" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="C9" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="D9" s="4" t="s">
         <v>150</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>153</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="42" customHeight="1">

</xml_diff>

<commit_message>
Updated Sphinx feature documentation
</commit_message>
<xml_diff>
--- a/docs/org.eclipse.sphinx.doc.design/excel/SphinxFeatureMap.xlsx
+++ b/docs/org.eclipse.sphinx.doc.design/excel/SphinxFeatureMap.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25596" windowHeight="13176"/>
   </bookViews>
   <sheets>
     <sheet name="Root Features" sheetId="4" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="191">
   <si>
     <t>Navigator &amp; Editor Sockets</t>
   </si>
@@ -394,9 +394,6 @@
     <t>Generic serialization/deserialization operating according to XML persistence Mapping annotations on underlying Ecore model. The XML persistence Mapping annotations are defined by Sphinx and extend the ExtendedMetaData annotations supported by EMF. They allow for a very flexible XML mappings of Ecore metamodels on a per-EStructuralFeature basis.</t>
   </si>
   <si>
-    <t>Provides generators for automatically adding XML Persistence Mapping annotations to Ecore metamodels and generating a corresponding XSD schema.</t>
-  </si>
-  <si>
     <t>Metamodel Generation</t>
   </si>
   <si>
@@ -404,9 +401,6 @@
   </si>
   <si>
     <t>org.eclipse.sphinx.emf.metamodelgen</t>
-  </si>
-  <si>
-    <t>Provides basic actions, command handlers and operations that are useful for implementing automatic metamodel generation tools.</t>
   </si>
   <si>
     <t>org.eclipse.sphinx.emf.metamodelgen
@@ -583,19 +577,6 @@
 org.eclipse.sphinx.emf.check.catalog.edit
 org.eclipse.sphinx.emf.check.catalog.editor
 org.eclipse.sphinx.emf.check.ui</t>
-  </si>
-  <si>
-    <t>org.eclipse.sphinx.core
-org.eclipse.sphinx.emf.check
-org.eclipse.sphinx.emf.editors.forms
-org.eclipse.sphinx.emf.metamodelgen
-org.eclipse.sphinx.emf.mwe.dynamic
-org.eclipse.sphinx.emf.navigators
-org.eclipse.sphinx.emf.serialization org.eclipse.sphinx.emf.serialization.generators
-org.eclipse.sphinx.emf.validation
-org.eclipse.sphinx.gmf.editors
-org.eclipse.sphinx.jdtpde
-org.eclipse.sphinx.xtendxpand</t>
   </si>
   <si>
     <t>Hummingbird metamodels and IDE integration including Model Explorer view contribution for Hummingbird content, generic Hummingbird form editor, exemplary graphical Hummingbird editors, exemplary model manipulation workflows for Hummingbird, exemplary validation services and constraints for Hummingbird, model transformation, code generation examples for Hummingbird and exemplary check validation and more.</t>
@@ -639,6 +620,55 @@
   <si>
     <t>org.eclipse.sphinx.examples.hummingbird10.incquery
 org.eclipse.sphinx.examples.hummingbird20.incquery</t>
+  </si>
+  <si>
+    <t>org.eclipse.sphinx.emf.editors</t>
+  </si>
+  <si>
+    <t>Compare &amp; Merge Integration</t>
+  </si>
+  <si>
+    <t>org.eclipse.sphinx.emf.compare</t>
+  </si>
+  <si>
+    <t>Sphinx EMF Compare Engine and Editor</t>
+  </si>
+  <si>
+    <t>org.eclipse.sphinx.emf.compare
+org.eclipse.sphinx.emf.compare.ui</t>
+  </si>
+  <si>
+    <t>Common logic for model editors that operate on indiviudal elements of Sphinx-managed shared model instances and integrate into the load/edit/save lifecycle of the same.</t>
+  </si>
+  <si>
+    <t>Common Editor Socket Logic</t>
+  </si>
+  <si>
+    <t>Sphinx Common Editor Socket Logic</t>
+  </si>
+  <si>
+    <t>Common logic for EMF Compare-based compare and merge editors that operate on indiviudal elements of Sphinx-managed shared model instances and integrate into the load/edit/save lifecycle of the same.</t>
+  </si>
+  <si>
+    <t>Basic actions, command handlers and operations that are useful for implementing automatic metamodel generation tools.</t>
+  </si>
+  <si>
+    <t>Generators for automatically adding XML Persistence Mapping annotations to Ecore metamodels and generating a corresponding XSD schema.</t>
+  </si>
+  <si>
+    <t>org.eclipse.sphinx.core
+org.eclipse.sphinx.emf.check
+org.eclipse.sphinx.emf.compare
+org.eclipse.sphinx.emf.editors
+org.eclipse.sphinx.emf.editors.forms
+org.eclipse.sphinx.emf.metamodelgen
+org.eclipse.sphinx.emf.mwe.dynamic
+org.eclipse.sphinx.emf.navigators
+org.eclipse.sphinx.emf.serialization org.eclipse.sphinx.emf.serialization.generators
+org.eclipse.sphinx.emf.validation
+org.eclipse.sphinx.gmf.editors
+org.eclipse.sphinx.jdtpde
+org.eclipse.sphinx.xtendxpand</t>
   </si>
 </sst>
 </file>
@@ -1012,8 +1042,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tableau3" displayName="Tableau3" ref="A1:F15" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
-  <autoFilter ref="A1:F15"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tableau3" displayName="Tableau3" ref="A1:F17" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
+  <autoFilter ref="A1:F17"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Top-level service" dataDxfId="11"/>
     <tableColumn id="2" name="Sub services" dataDxfId="10"/>
@@ -1331,22 +1361,22 @@
   </sheetPr>
   <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="31" style="4" customWidth="1"/>
     <col min="2" max="2" width="30.33203125" style="4" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="35" style="4" customWidth="1"/>
-    <col min="4" max="4" width="42.5" style="4" customWidth="1"/>
-    <col min="5" max="5" width="48.83203125" style="6" customWidth="1"/>
+    <col min="4" max="4" width="42.44140625" style="4" customWidth="1"/>
+    <col min="5" max="5" width="48.77734375" style="6" customWidth="1"/>
     <col min="6" max="6" width="34.6640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.83203125" style="4"/>
+    <col min="7" max="16384" width="8.77734375" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="5" customFormat="1">
+    <row r="1" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>42</v>
       </c>
@@ -1366,7 +1396,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="149" customHeight="1">
+    <row r="2" spans="1:6" ht="177.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>16</v>
       </c>
@@ -1376,14 +1406,14 @@
       <c r="C2" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="E2" s="4" t="s">
-        <v>172</v>
+      <c r="E2" s="9" t="s">
+        <v>190</v>
       </c>
       <c r="F2" s="7" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="24">
+    <row r="3" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>36</v>
       </c>
@@ -1400,7 +1430,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>38</v>
       </c>
@@ -1418,7 +1448,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="36">
+    <row r="5" spans="1:6" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>17</v>
       </c>
@@ -1435,58 +1465,58 @@
         <v>89</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="46" customHeight="1">
+    <row r="6" spans="1:6" ht="46.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C6" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="46.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>166</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E7" s="4" t="s">
         <v>160</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="46" customHeight="1">
-      <c r="A7" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>155</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>168</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>162</v>
       </c>
       <c r="F7" s="7" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="46" customHeight="1">
+    <row r="8" spans="1:6" ht="46.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="E8" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="F8" s="7" t="s">
         <v>161</v>
       </c>
-      <c r="F8" s="7" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="36">
+    </row>
+    <row r="9" spans="1:6" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>91</v>
       </c>
@@ -1500,10 +1530,10 @@
         <v>66</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="24">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>92</v>
       </c>
@@ -1520,7 +1550,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="36">
+    <row r="11" spans="1:6" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>90</v>
       </c>
@@ -1532,10 +1562,10 @@
       </c>
       <c r="E11" s="4"/>
       <c r="F11" s="7" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="122" customHeight="1">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="121.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>18</v>
       </c>
@@ -1546,47 +1576,47 @@
         <v>83</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="F12" s="7" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="46" customHeight="1">
+    <row r="13" spans="1:6" ht="46.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E13" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="46.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="F13" s="7" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="46" customHeight="1">
-      <c r="A14" s="4" t="s">
+      <c r="B14" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="E14" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="B14" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>158</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>148</v>
-      </c>
       <c r="F14" s="7" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="52.5" customHeight="1">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>19</v>
       </c>
@@ -1604,7 +1634,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="84">
+    <row r="16" spans="1:6" ht="92.4" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>20</v>
       </c>
@@ -1643,24 +1673,24 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <outlinePr summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.83203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.1640625" style="4" customWidth="1"/>
+    <col min="1" max="1" width="26.77734375" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.109375" style="4" customWidth="1"/>
     <col min="3" max="3" width="40" style="4" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="33.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="47.5" style="4" customWidth="1"/>
-    <col min="6" max="6" width="40.83203125" style="4" customWidth="1"/>
-    <col min="7" max="16384" width="8.83203125" style="4"/>
+    <col min="5" max="5" width="47.44140625" style="4" customWidth="1"/>
+    <col min="6" max="6" width="40.77734375" style="4" customWidth="1"/>
+    <col min="7" max="16384" width="8.77734375" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="5" customFormat="1">
+    <row r="1" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>5</v>
       </c>
@@ -1680,7 +1710,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="36">
+    <row r="2" spans="1:6" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
@@ -1700,261 +1730,298 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="36">
+    <row r="3" spans="1:6" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>10</v>
+      <c r="B3" s="9" t="s">
+        <v>185</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>72</v>
+        <v>179</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>184</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="24">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>121</v>
+        <v>10</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>66</v>
+        <v>6</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="48">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B5" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="52.8" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C6" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D6" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E6" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="F6" s="4" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="43" customHeight="1">
-      <c r="A6" s="4" t="s">
+    <row r="7" spans="1:6" ht="43.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="E7" s="4" t="s">
         <v>174</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="F7" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="66" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="E8" s="4" t="s">
         <v>175</v>
       </c>
-      <c r="C6" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>176</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>177</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="60">
-      <c r="A7" s="4" t="s">
-        <v>174</v>
-      </c>
-      <c r="B7" s="4" t="s">
+      <c r="F8" s="4" t="s">
         <v>169</v>
       </c>
-      <c r="C7" s="4" t="s">
-        <v>170</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>180</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>178</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="38" customHeight="1">
-      <c r="A8" s="4" t="s">
-        <v>159</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>160</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="48">
+    </row>
+    <row r="9" spans="1:6" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="52.8" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="66" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B11" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="B9" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="D9" s="9" t="s">
-        <v>126</v>
-      </c>
-      <c r="E9" s="9" t="s">
-        <v>128</v>
-      </c>
-      <c r="F9" s="9" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="60">
-      <c r="A10" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="C10" s="4" t="s">
+      <c r="C11" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D11" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="E11" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="F10" s="11" t="s">
+      <c r="F11" s="11" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="36">
-      <c r="A11" s="4" t="s">
+    <row r="12" spans="1:6" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="D12" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="E12" s="9" t="s">
+        <v>188</v>
+      </c>
+      <c r="F12" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="D11" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="24">
-      <c r="A12" s="4" t="s">
+    </row>
+    <row r="13" spans="1:6" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="D13" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="E13" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="F13" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="E12" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="84">
-      <c r="A13" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="36">
+    </row>
+    <row r="14" spans="1:6" ht="92.4" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>106</v>
       </c>
       <c r="B14" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="B15" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C15" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="D15" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="E14" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="F14" s="4" t="s">
+      <c r="E15" s="9" t="s">
+        <v>189</v>
+      </c>
+      <c r="F15" s="4" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="87.75" customHeight="1">
-      <c r="A15" s="4" t="s">
+    <row r="16" spans="1:6" ht="52.8" x14ac:dyDescent="0.25">
+      <c r="A16" s="9" t="s">
+        <v>180</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="E16" s="9" t="s">
+        <v>187</v>
+      </c>
+      <c r="F16" s="9" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="87.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B15" s="9" t="s">
+      <c r="B17" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C17" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="D17" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="E15" s="4" t="s">
+      <c r="E17" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="F15" s="9" t="s">
+      <c r="F17" s="9" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="20" spans="6:6">
-      <c r="F20" s="8"/>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F22" s="8"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.78740157499999996" right="0.78740157499999996" top="0.984251969" bottom="0.984251969" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
@@ -1971,20 +2038,20 @@
   </sheetPr>
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="49.33203125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="31.1640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="31.109375" style="1" customWidth="1"/>
     <col min="3" max="3" width="43" style="1" customWidth="1"/>
-    <col min="4" max="4" width="61.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.83203125" customWidth="1"/>
+    <col min="4" max="4" width="61.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="2" customFormat="1">
+    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>42</v>
       </c>
@@ -1999,7 +2066,7 @@
       </c>
       <c r="E1" s="3"/>
     </row>
-    <row r="2" spans="1:5" ht="24">
+    <row r="2" spans="1:5" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>30</v>
       </c>
@@ -2013,7 +2080,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>26</v>
       </c>
@@ -2027,21 +2094,21 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="24">
+    <row r="4" spans="1:5" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B4" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>131</v>
-      </c>
       <c r="D4" s="4" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="36">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>28</v>
       </c>
@@ -2055,7 +2122,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="48">
+    <row r="6" spans="1:5" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>27</v>
       </c>
@@ -2069,7 +2136,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="207" customHeight="1">
+    <row r="7" spans="1:5" ht="207" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>32</v>
       </c>
@@ -2077,41 +2144,41 @@
         <v>63</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="48" customHeight="1">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="32" customHeight="1">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="31.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="D9" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="B9" s="4" t="s">
-        <v>149</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>152</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="42" customHeight="1">
+    </row>
+    <row r="10" spans="1:5" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>33</v>
       </c>
@@ -2125,7 +2192,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="56" customHeight="1">
+    <row r="11" spans="1:5" ht="55.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>34</v>
       </c>
@@ -2136,7 +2203,7 @@
         <v>80</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[ASSIGNED] Bug 458637 - EMF Model Search https://bugs.eclipse.org/bugs/show_bug.cgi?id=458637
Added Sphinx search features and updates docs.
</commit_message>
<xml_diff>
--- a/docs/org.eclipse.sphinx.doc.design/excel/SphinxFeatureMap.xlsx
+++ b/docs/org.eclipse.sphinx.doc.design/excel/SphinxFeatureMap.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25596" windowHeight="13176"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="13180" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Root Features" sheetId="4" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="196">
   <si>
     <t>Navigator &amp; Editor Sockets</t>
   </si>
@@ -551,10 +551,6 @@
   </si>
   <si>
     <t>Sphinx Nebula</t>
-  </si>
-  <si>
-    <t>org.eclipse.sphinx.emf.incquery
-org.eclipse.sphinx.emf.workspace.incquery</t>
   </si>
   <si>
     <t>Includes runtime binaries of Sphinx extensions for EMF-IncQuery (without source code).</t>
@@ -656,6 +652,23 @@
     <t>Generators for automatically adding XML Persistence Mapping annotations to Ecore metamodels and generating a corresponding XSD schema.</t>
   </si>
   <si>
+    <t>Model Search</t>
+  </si>
+  <si>
+    <t>org.eclipse.sphinx.emf.search</t>
+  </si>
+  <si>
+    <t>Sphinx EMF Search</t>
+  </si>
+  <si>
+    <t>org.eclipse.sphinx.emf.search.ui</t>
+  </si>
+  <si>
+    <t>org.eclipse.sphinx.emf.incquery
+org.eclipse.sphinx.emf.workspace.incquery
+org.eclipse.sphinx.emf.search.ui.incquery</t>
+  </si>
+  <si>
     <t>org.eclipse.sphinx.core
 org.eclipse.sphinx.emf.check
 org.eclipse.sphinx.emf.compare
@@ -664,11 +677,15 @@
 org.eclipse.sphinx.emf.metamodelgen
 org.eclipse.sphinx.emf.mwe.dynamic
 org.eclipse.sphinx.emf.navigators
+org.eclipse.sphinx.emf.search
 org.eclipse.sphinx.emf.serialization org.eclipse.sphinx.emf.serialization.generators
 org.eclipse.sphinx.emf.validation
 org.eclipse.sphinx.gmf.editors
 org.eclipse.sphinx.jdtpde
 org.eclipse.sphinx.xtendxpand</t>
+  </si>
+  <si>
+    <t>Model Search allow to find occurrences of model objects with integration in the Eclipse Search framework. Searching is supported by an index that is contributed for each meta-model and is kept up to date in the background as the resources are changed.</t>
   </si>
 </sst>
 </file>
@@ -1042,8 +1059,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tableau3" displayName="Tableau3" ref="A1:F17" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
-  <autoFilter ref="A1:F17"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tableau3" displayName="Tableau3" ref="A1:F18" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
+  <autoFilter ref="A1:F18"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Top-level service" dataDxfId="11"/>
     <tableColumn id="2" name="Sub services" dataDxfId="10"/>
@@ -1361,22 +1378,22 @@
   </sheetPr>
   <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="31" style="4" customWidth="1"/>
     <col min="2" max="2" width="30.33203125" style="4" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="35" style="4" customWidth="1"/>
-    <col min="4" max="4" width="42.44140625" style="4" customWidth="1"/>
-    <col min="5" max="5" width="48.77734375" style="6" customWidth="1"/>
+    <col min="4" max="4" width="42.5" style="4" customWidth="1"/>
+    <col min="5" max="5" width="48.83203125" style="6" customWidth="1"/>
     <col min="6" max="6" width="34.6640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.77734375" style="4"/>
+    <col min="7" max="16384" width="8.83203125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="5" customFormat="1">
       <c r="A1" s="4" t="s">
         <v>42</v>
       </c>
@@ -1396,7 +1413,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="177.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="188" customHeight="1">
       <c r="A2" s="4" t="s">
         <v>16</v>
       </c>
@@ -1406,14 +1423,14 @@
       <c r="C2" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="E2" s="9" t="s">
-        <v>190</v>
+      <c r="E2" s="11" t="s">
+        <v>194</v>
       </c>
       <c r="F2" s="7" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="24">
       <c r="A3" s="4" t="s">
         <v>36</v>
       </c>
@@ -1430,7 +1447,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6">
       <c r="A4" s="4" t="s">
         <v>38</v>
       </c>
@@ -1448,7 +1465,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="36">
       <c r="A5" s="4" t="s">
         <v>17</v>
       </c>
@@ -1465,7 +1482,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="46.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="46" customHeight="1">
       <c r="A6" s="4" t="s">
         <v>138</v>
       </c>
@@ -1473,7 +1490,7 @@
         <v>152</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>158</v>
@@ -1482,7 +1499,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="46.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="46" customHeight="1">
       <c r="A7" s="4" t="s">
         <v>139</v>
       </c>
@@ -1490,7 +1507,7 @@
         <v>153</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>160</v>
@@ -1499,7 +1516,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="46.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="46" customHeight="1">
       <c r="A8" s="4" t="s">
         <v>140</v>
       </c>
@@ -1507,7 +1524,7 @@
         <v>154</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>159</v>
@@ -1516,7 +1533,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="36">
       <c r="A9" s="4" t="s">
         <v>91</v>
       </c>
@@ -1533,7 +1550,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="24">
       <c r="A10" s="4" t="s">
         <v>92</v>
       </c>
@@ -1550,7 +1567,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="36">
       <c r="A11" s="4" t="s">
         <v>90</v>
       </c>
@@ -1565,7 +1582,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="121.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="122" customHeight="1">
       <c r="A12" s="4" t="s">
         <v>18</v>
       </c>
@@ -1582,7 +1599,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="46.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="46" customHeight="1">
       <c r="A13" s="4" t="s">
         <v>141</v>
       </c>
@@ -1599,7 +1616,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="46.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="46" customHeight="1">
       <c r="A14" s="4" t="s">
         <v>144</v>
       </c>
@@ -1616,7 +1633,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="52.5" customHeight="1">
       <c r="A15" s="4" t="s">
         <v>19</v>
       </c>
@@ -1634,7 +1651,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="92.4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="84">
       <c r="A16" s="4" t="s">
         <v>20</v>
       </c>
@@ -1673,24 +1690,24 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <outlinePr summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="26.77734375" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.109375" style="4" customWidth="1"/>
+    <col min="1" max="1" width="26.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.1640625" style="4" customWidth="1"/>
     <col min="3" max="3" width="40" style="4" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="33.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="47.44140625" style="4" customWidth="1"/>
-    <col min="6" max="6" width="40.77734375" style="4" customWidth="1"/>
-    <col min="7" max="16384" width="8.77734375" style="4"/>
+    <col min="5" max="5" width="47.5" style="4" customWidth="1"/>
+    <col min="6" max="6" width="40.83203125" style="4" customWidth="1"/>
+    <col min="7" max="16384" width="8.83203125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="5" customFormat="1">
       <c r="A1" s="4" t="s">
         <v>5</v>
       </c>
@@ -1710,7 +1727,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="36">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
@@ -1730,27 +1747,27 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="52.8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="36">
       <c r="A3" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="9" t="s">
+        <v>184</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="D3" s="9" t="s">
         <v>185</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>179</v>
-      </c>
-      <c r="D3" s="9" t="s">
-        <v>186</v>
-      </c>
       <c r="E3" s="9" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="52.8" x14ac:dyDescent="0.25">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="36">
       <c r="A4" s="4" t="s">
         <v>0</v>
       </c>
@@ -1770,7 +1787,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="24">
       <c r="A5" s="4" t="s">
         <v>0</v>
       </c>
@@ -1790,7 +1807,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="52.8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="48">
       <c r="A6" s="4" t="s">
         <v>0</v>
       </c>
@@ -1810,47 +1827,47 @@
         <v>69</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="43.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="43" customHeight="1">
       <c r="A7" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>171</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>172</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D7" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="E7" s="4" t="s">
         <v>173</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>174</v>
       </c>
       <c r="F7" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="66" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="60">
       <c r="A8" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B8" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="C8" s="4" t="s">
         <v>167</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="D8" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="F8" s="4" t="s">
         <v>168</v>
       </c>
-      <c r="D8" s="4" t="s">
-        <v>177</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>175</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:6" ht="38" customHeight="1">
       <c r="A9" s="4" t="s">
         <v>157</v>
       </c>
@@ -1858,10 +1875,10 @@
         <v>158</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="52.8" x14ac:dyDescent="0.25">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="48">
       <c r="A10" s="4" t="s">
         <v>121</v>
       </c>
@@ -1881,7 +1898,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="66" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="60">
       <c r="A11" s="4" t="s">
         <v>53</v>
       </c>
@@ -1901,7 +1918,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="36">
       <c r="A12" s="4" t="s">
         <v>115</v>
       </c>
@@ -1912,13 +1929,13 @@
         <v>116</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F12" s="4" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="24">
       <c r="A13" s="4" t="s">
         <v>131</v>
       </c>
@@ -1935,7 +1952,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="92.4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="84">
       <c r="A14" s="4" t="s">
         <v>106</v>
       </c>
@@ -1955,7 +1972,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="36">
       <c r="A15" s="4" t="s">
         <v>106</v>
       </c>
@@ -1969,59 +1986,76 @@
         <v>112</v>
       </c>
       <c r="E15" s="9" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="F15" s="4" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="52.8" x14ac:dyDescent="0.25">
-      <c r="A16" s="9" t="s">
+    <row r="16" spans="1:6" ht="73" customHeight="1">
+      <c r="A16" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="E16" s="11" t="s">
+        <v>195</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="48">
+      <c r="A17" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="C17" s="9" t="s">
         <v>180</v>
       </c>
-      <c r="C16" s="9" t="s">
+      <c r="D17" s="9" t="s">
         <v>181</v>
       </c>
-      <c r="D16" s="9" t="s">
+      <c r="E17" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="F17" s="9" t="s">
         <v>182</v>
       </c>
-      <c r="E16" s="9" t="s">
-        <v>187</v>
-      </c>
-      <c r="F16" s="9" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="87.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
+    </row>
+    <row r="18" spans="1:6" ht="87.75" customHeight="1">
+      <c r="A18" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B17" s="9" t="s">
+      <c r="B18" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="C18" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D17" s="4" t="s">
+      <c r="D18" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="E17" s="4" t="s">
+      <c r="E18" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="F17" s="9" t="s">
+      <c r="F18" s="9" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F22" s="8"/>
+    <row r="23" spans="1:6">
+      <c r="F23" s="8"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.78740157499999996" right="0.78740157499999996" top="0.984251969" bottom="0.984251969" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter alignWithMargins="0"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId1"/>
   </tableParts>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
@@ -2042,16 +2076,16 @@
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="49.33203125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="31.109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="31.1640625" style="1" customWidth="1"/>
     <col min="3" max="3" width="43" style="1" customWidth="1"/>
-    <col min="4" max="4" width="61.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.77734375" customWidth="1"/>
+    <col min="4" max="4" width="61.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" s="2" customFormat="1">
       <c r="A1" s="4" t="s">
         <v>42</v>
       </c>
@@ -2066,7 +2100,7 @@
       </c>
       <c r="E1" s="3"/>
     </row>
-    <row r="2" spans="1:5" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="24">
       <c r="A2" s="4" t="s">
         <v>30</v>
       </c>
@@ -2080,7 +2114,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3" s="4" t="s">
         <v>26</v>
       </c>
@@ -2094,7 +2128,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="24">
       <c r="A4" s="4" t="s">
         <v>128</v>
       </c>
@@ -2108,7 +2142,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="36">
       <c r="A5" s="4" t="s">
         <v>28</v>
       </c>
@@ -2122,7 +2156,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="52.8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="48">
       <c r="A6" s="4" t="s">
         <v>27</v>
       </c>
@@ -2136,7 +2170,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="207" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="207" customHeight="1">
       <c r="A7" s="4" t="s">
         <v>32</v>
       </c>
@@ -2144,13 +2178,13 @@
         <v>63</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="48" customHeight="1">
       <c r="A8" s="4" t="s">
         <v>142</v>
       </c>
@@ -2161,10 +2195,10 @@
         <v>149</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="31.95" customHeight="1" x14ac:dyDescent="0.25">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="32" customHeight="1">
       <c r="A9" s="4" t="s">
         <v>146</v>
       </c>
@@ -2178,7 +2212,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="42" customHeight="1">
       <c r="A10" s="4" t="s">
         <v>33</v>
       </c>
@@ -2192,7 +2226,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="55.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="56" customHeight="1">
       <c r="A11" s="4" t="s">
         <v>34</v>
       </c>

</xml_diff>

<commit_message>
RESOVLED - bug 487564: Provide a reusable base implementation of an IURIChangeDetectorDelegate for URIs with hierarchical fragments https://bugs.eclipse.org/bugs/show_bug.cgi?id=487564
</commit_message>
<xml_diff>
--- a/docs/org.eclipse.sphinx.doc.design/excel/SphinxFeatureMap.xlsx
+++ b/docs/org.eclipse.sphinx.doc.design/excel/SphinxFeatureMap.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\eclipse-sphinx\org.eclipse.sphinx\docs\org.eclipse.sphinx.doc.design\excel\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="13180" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="13185" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Root Features" sheetId="4" r:id="rId1"/>
@@ -593,24 +598,6 @@
     <t>Annotation-based framework for validating EMF models.</t>
   </si>
   <si>
-    <t>org.eclipse.sphinx.examples.hummingbird.ide
-org.eclipse.sphinx.examples.hummingbird.ide.ui
-org.eclipse.sphinx.examples.hummingbird10
-org.eclipse.sphinx.examples.hummingbird10.edit
-org.eclipse.sphinx.examples.hummingbird10.ide.ui
-org.eclipse.sphinx.examples.hummingbird.metamodelgen
-org.eclipse.sphinx.examples.hummingbird.metamodelgen.ui
-org.eclipse.sphinx.examples.hummingbird20
-org.eclipse.sphinx.examples.hummingbird20.codegen.xpand.newwizard
-org.eclipse.sphinx.examples.hummingbird20.diagram.gmf
-org.eclipse.sphinx.examples.hummingbird20.edit
-org.eclipse.sphinx.examples.hummingbird20.ide.ui
-org.eclipse.sphinx.examples.hummingbird20.transform.xtend.newwizard
-org.eclipse.sphinx.examples.hummingbird20.validation
-org.eclipse.sphinx.examples.hummingbird20.check
-org.eclipse.sphinx.examples.hummingbird20.workflows.newwizard</t>
-  </si>
-  <si>
     <t>Sphinx EMF Check Validation</t>
   </si>
   <si>
@@ -687,11 +674,33 @@
   <si>
     <t>Model Search allow to find occurrences of model objects with integration in the Eclipse Search framework. Searching is supported by an index that is contributed for each meta-model and is kept up to date in the background as the resources are changed.</t>
   </si>
+  <si>
+    <t>org.eclipse.sphinx.examples.hummingbird.ide
+org.eclipse.sphinx.examples.hummingbird.ide.ui
+org.eclipse.sphinx.examples.hummingbird.metamodelgen
+org.eclipse.sphinx.examples.hummingbird.metamodelgen.ui
+org.eclipse.sphinx.examples.hummingbird10
+org.eclipse.sphinx.examples.hummingbird10.edit
+org.eclipse.sphinx.examples.hummingbird10.ide.ui
+org.eclipse.sphinx.examples.hummingbird20
+org.eclipse.sphinx.examples.hummingbird20.check
+org.eclipse.sphinx.examples.hummingbird20.codegen.xpand.newwizard
+org.eclipse.sphinx.examples.hummingbird20.diagram.gmf
+org.eclipse.sphinx.examples.hummingbird20.edit
+org.eclipse.sphinx.examples.hummingbird20.emf.compare
+org.eclipse.sphinx.examples.hummingbird20.ide
+org.eclipse.sphinx.examples.hummingbird20.ide.ui
+org.eclipse.sphinx.examples.hummingbird20.splitting
+org.eclipse.sphinx.examples.hummingbird20.splitting.ui
+org.eclipse.sphinx.examples.hummingbird20.transform.xtend.newwizard
+org.eclipse.sphinx.examples.hummingbird20.validation
+org.eclipse.sphinx.examples.hummingbird20.workflows.newwizard</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -1373,7 +1382,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+  <sheetPr>
     <outlinePr summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:F16"/>
@@ -1382,18 +1391,18 @@
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="31" style="4" customWidth="1"/>
-    <col min="2" max="2" width="30.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.28515625" style="4" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="35" style="4" customWidth="1"/>
-    <col min="4" max="4" width="42.5" style="4" customWidth="1"/>
-    <col min="5" max="5" width="48.83203125" style="6" customWidth="1"/>
-    <col min="6" max="6" width="34.6640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.83203125" style="4"/>
+    <col min="4" max="4" width="42.42578125" style="4" customWidth="1"/>
+    <col min="5" max="5" width="48.85546875" style="6" customWidth="1"/>
+    <col min="6" max="6" width="34.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.85546875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="5" customFormat="1">
+    <row r="1" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>42</v>
       </c>
@@ -1413,7 +1422,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="188" customHeight="1">
+    <row r="2" spans="1:6" ht="188.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>16</v>
       </c>
@@ -1424,13 +1433,13 @@
         <v>81</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="F2" s="7" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="24">
+    <row r="3" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>36</v>
       </c>
@@ -1447,7 +1456,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>38</v>
       </c>
@@ -1465,7 +1474,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="36">
+    <row r="5" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>17</v>
       </c>
@@ -1482,7 +1491,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="46" customHeight="1">
+    <row r="6" spans="1:6" ht="45.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>138</v>
       </c>
@@ -1499,7 +1508,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="46" customHeight="1">
+    <row r="7" spans="1:6" ht="45.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>139</v>
       </c>
@@ -1516,7 +1525,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="46" customHeight="1">
+    <row r="8" spans="1:6" ht="45.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>140</v>
       </c>
@@ -1533,7 +1542,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="36">
+    <row r="9" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>91</v>
       </c>
@@ -1550,7 +1559,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="24">
+    <row r="10" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>92</v>
       </c>
@@ -1567,7 +1576,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="36">
+    <row r="11" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>90</v>
       </c>
@@ -1582,7 +1591,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="122" customHeight="1">
+    <row r="12" spans="1:6" ht="122.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
         <v>18</v>
       </c>
@@ -1599,7 +1608,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="46" customHeight="1">
+    <row r="13" spans="1:6" ht="45.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
         <v>141</v>
       </c>
@@ -1616,7 +1625,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="46" customHeight="1">
+    <row r="14" spans="1:6" ht="45.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>144</v>
       </c>
@@ -1633,7 +1642,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="52.5" customHeight="1">
+    <row r="15" spans="1:6" ht="52.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
         <v>19</v>
       </c>
@@ -1651,7 +1660,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="84">
+    <row r="16" spans="1:6" ht="89.25" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
         <v>20</v>
       </c>
@@ -1687,27 +1696,27 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+  <sheetPr>
     <outlinePr summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="26.83203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.1640625" style="4" customWidth="1"/>
+    <col min="1" max="1" width="26.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.140625" style="4" customWidth="1"/>
     <col min="3" max="3" width="40" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="33.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="47.5" style="4" customWidth="1"/>
-    <col min="6" max="6" width="40.83203125" style="4" customWidth="1"/>
-    <col min="7" max="16384" width="8.83203125" style="4"/>
+    <col min="4" max="4" width="33.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="47.42578125" style="4" customWidth="1"/>
+    <col min="6" max="6" width="40.85546875" style="4" customWidth="1"/>
+    <col min="7" max="16384" width="8.85546875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="5" customFormat="1">
+    <row r="1" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>5</v>
       </c>
@@ -1727,7 +1736,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="36">
+    <row r="2" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
@@ -1747,27 +1756,27 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="36">
+    <row r="3" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="9" t="s">
+        <v>183</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="D3" s="9" t="s">
         <v>184</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>178</v>
-      </c>
-      <c r="D3" s="9" t="s">
-        <v>185</v>
-      </c>
       <c r="E3" s="9" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="36">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>0</v>
       </c>
@@ -1787,7 +1796,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="24">
+    <row r="5" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>0</v>
       </c>
@@ -1807,7 +1816,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="48">
+    <row r="6" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>0</v>
       </c>
@@ -1827,7 +1836,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="43" customHeight="1">
+    <row r="7" spans="1:6" ht="42.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>170</v>
       </c>
@@ -1847,7 +1856,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="60">
+    <row r="8" spans="1:6" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>170</v>
       </c>
@@ -1858,7 +1867,7 @@
         <v>167</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>174</v>
@@ -1867,7 +1876,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="38" customHeight="1">
+    <row r="9" spans="1:6" ht="38.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>157</v>
       </c>
@@ -1875,10 +1884,10 @@
         <v>158</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="48">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>121</v>
       </c>
@@ -1898,7 +1907,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="60">
+    <row r="11" spans="1:6" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>53</v>
       </c>
@@ -1918,7 +1927,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="36">
+    <row r="12" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
         <v>115</v>
       </c>
@@ -1929,13 +1938,13 @@
         <v>116</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="F12" s="4" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="24">
+    <row r="13" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
         <v>131</v>
       </c>
@@ -1952,7 +1961,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="84">
+    <row r="14" spans="1:6" ht="89.25" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>106</v>
       </c>
@@ -1972,7 +1981,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="36">
+    <row r="15" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
         <v>106</v>
       </c>
@@ -1986,47 +1995,47 @@
         <v>112</v>
       </c>
       <c r="E15" s="9" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F15" s="4" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="73" customHeight="1">
+    <row r="16" spans="1:6" ht="72.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="C16" s="4" t="s">
         <v>189</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="D16" s="4" t="s">
         <v>190</v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="E16" s="11" t="s">
+        <v>194</v>
+      </c>
+      <c r="F16" s="4" t="s">
         <v>191</v>
       </c>
-      <c r="E16" s="11" t="s">
-        <v>195</v>
-      </c>
-      <c r="F16" s="4" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="48">
+    </row>
+    <row r="17" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A17" s="9" t="s">
+        <v>178</v>
+      </c>
+      <c r="C17" s="9" t="s">
         <v>179</v>
       </c>
-      <c r="C17" s="9" t="s">
+      <c r="D17" s="9" t="s">
         <v>180</v>
       </c>
-      <c r="D17" s="9" t="s">
+      <c r="E17" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="F17" s="9" t="s">
         <v>181</v>
       </c>
-      <c r="E17" s="9" t="s">
-        <v>186</v>
-      </c>
-      <c r="F17" s="9" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="87.75" customHeight="1">
+    </row>
+    <row r="18" spans="1:6" ht="87.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
         <v>1</v>
       </c>
@@ -2046,7 +2055,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="F23" s="8"/>
     </row>
   </sheetData>
@@ -2067,25 +2076,25 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+  <sheetPr>
     <outlinePr summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="49.33203125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="31.1640625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="49.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="31.140625" style="1" customWidth="1"/>
     <col min="3" max="3" width="43" style="1" customWidth="1"/>
-    <col min="4" max="4" width="61.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.83203125" customWidth="1"/>
+    <col min="4" max="4" width="61.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="2" customFormat="1">
+    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>42</v>
       </c>
@@ -2100,7 +2109,7 @@
       </c>
       <c r="E1" s="3"/>
     </row>
-    <row r="2" spans="1:5" ht="24">
+    <row r="2" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>30</v>
       </c>
@@ -2114,7 +2123,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>26</v>
       </c>
@@ -2128,7 +2137,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="24">
+    <row r="4" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>128</v>
       </c>
@@ -2142,7 +2151,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="36">
+    <row r="5" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>28</v>
       </c>
@@ -2156,7 +2165,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="48">
+    <row r="6" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>27</v>
       </c>
@@ -2170,7 +2179,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="207" customHeight="1">
+    <row r="7" spans="1:5" ht="267.75" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>32</v>
       </c>
@@ -2181,10 +2190,10 @@
         <v>169</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="48" customHeight="1">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="48" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>142</v>
       </c>
@@ -2195,10 +2204,10 @@
         <v>149</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="32" customHeight="1">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="32.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>146</v>
       </c>
@@ -2212,7 +2221,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="42" customHeight="1">
+    <row r="10" spans="1:5" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>33</v>
       </c>
@@ -2226,7 +2235,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="56" customHeight="1">
+    <row r="11" spans="1:5" ht="56.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>34</v>
       </c>

</xml_diff>